<commit_message>
Added code for both the sheets, raw and cleaned
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,13 +8,317 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="316">
+  <si>
+    <t>AllData</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Ice Cream, Coffee and Tea', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16843901_CHAIN_1e4f81766802ac0aa1392816deedacb3_c.png', u'average_cost_for_two': 25, u'deeplink': u'zomato://restaurant/16843902', u'id': u'16843902', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16843901_CHAIN_1e4f81766802ac0aa1392816deedacb3_c.png?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/ghirardelli-ice-cream-and-chocolate-shop-fishermans-wharf/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/ghirardelli-ice-cream-and-chocolate-shop-fishermans-wharf/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'418', u'aggregate_rating': u'4.9', u'rating_text': u'Excellent', u'rating_color': u'3F7E00'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Ghiradelli Square', u'city_id': 306, u'country_id': 216, u'zipcode': u'94109', u'longitude': u'-122.4222722222', u'address': u'Ghirardelli Square, 900 North Point Street, San Francisco 94109', u'latitude': u'37.8058083333', u'locality_verbose': u'Ghiradelli Square, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/ghirardelli-ice-cream-and-chocolate-shop-fishermans-wharf/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16843902}, u'price_range': 1, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Ghirardelli Ice Cream and Chocolate Shop', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/ghirardelli-ice-cream-and-chocolate-shop-fishermans-wharf?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Vietnamese, Fusion', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16850231_RESTAURANT_c080883c4b17b47ff0c9cdaa96462318_c.png', u'average_cost_for_two': 100, u'deeplink': u'zomato://restaurant/16850231', u'id': u'16850231', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16850231_RESTAURANT_c080883c4b17b47ff0c9cdaa96462318_c.png?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/the-slanted-door-embarcadero/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/the-slanted-door-embarcadero/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'2022', u'aggregate_rating': u'4.5', u'rating_text': u'Excellent', u'rating_color': u'3F7E00'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Ferry Building ', u'city_id': 306, u'country_id': 216, u'zipcode': u'94111', u'longitude': u'-122.3936777778', u'address': u'Ferry Building, Level 1, 1 Ferry Plaza, Suite 5, San Francisco 94111', u'latitude': u'37.7962638889', u'locality_verbose': u'Ferry Building , San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/the-slanted-door-embarcadero/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16850231}, u'price_range': 4, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'The Slanted Door', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/the-slanted-door-embarcadero?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Italian, French, California', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16852971_RESTAURANT_ed414bd9d75c685b2e8b6982cd928a9a_c.jpg', u'average_cost_for_two': 90, u'deeplink': u'zomato://restaurant/16852971', u'id': u'16852971', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16852971_RESTAURANT_ed414bd9d75c685b2e8b6982cd928a9a_c.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/zuni-caf\xe9-civic-center/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/zuni-caf\xe9-civic-center/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'1062', u'aggregate_rating': u'4.3', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Civic Center', u'city_id': 306, u'country_id': 216, u'zipcode': u'94102', u'longitude': u'-122.4213638889', u'address': u'1658 Market Street, San Francisco 94102', u'latitude': u'37.7736888889', u'locality_verbose': u'Civic Center, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/zuni-caf\xe9-civic-center/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16852971}, u'price_range': 3, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Zuni Caf\xe9', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/zuni-caf\xe9-civic-center?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Cafe, Bakery', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16840976_RESTAURANT_49346c02943c5acf521269e136524a15_c.JPG?output-format=webp', u'average_cost_for_two': 25, u'deeplink': u'zomato://restaurant/16840976', u'id': u'16840976', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16840976_RESTAURANT_49346c02943c5acf521269e136524a15_c.JPG?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/boudin-bakery-fishermans-wharf/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/boudin-bakery-fishermans-wharf/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'496', u'aggregate_rating': u'4.5', u'rating_text': u'Excellent', u'rating_color': u'3F7E00'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u"Fisherman's Wharf", u'city_id': 306, u'country_id': 216, u'zipcode': u'94133', u'longitude': u'-122.4146440000', u'address': u'160 Jefferson Street, San Francisco 94133', u'latitude': u'37.8087800000', u'locality_verbose': u"Fisherman's Wharf, San Francisco"}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/boudin-bakery-fishermans-wharf/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16840976}, u'price_range': 1, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Boudin Bakery', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/boudin-bakery-fishermans-wharf?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Cajun, Southern', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16853056_RESTAURANT_2ea23688d207d78fae14a2bce5a7ee7c.png?output-format=webp', u'average_cost_for_two': 40, u'deeplink': u'zomato://restaurant/16853056', u'id': u'16853056', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16853056_RESTAURANT_2ea23688d207d78fae14a2bce5a7ee7c.png?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/brendas-french-soul-food-civic-center/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/brendas-french-soul-food-civic-center/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'794', u'aggregate_rating': u'4.6', u'rating_text': u'Excellent', u'rating_color': u'3F7E00'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Civic Center', u'city_id': 306, u'country_id': 216, u'zipcode': u'94102', u'longitude': u'-122.4187690000', u'address': u'652 Polk Street, San Francisco 94102', u'latitude': u'37.7829200000', u'locality_verbose': u'Civic Center, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/brendas-french-soul-food-civic-center/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16853056}, u'price_range': 2, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u"Brenda's French Soul Food", u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/brendas-french-soul-food-civic-center?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Seafood', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16844513_RESTAURANT_3e410b27cb6812ac2abfb39dffe379da_c.jpg', u'average_cost_for_two': 120, u'deeplink': u'zomato://restaurant/16844513', u'id': u'16844513', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16844513_RESTAURANT_3e410b27cb6812ac2abfb39dffe379da_c.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/hog-island-oyster-company-embarcadero/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/hog-island-oyster-company-embarcadero/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'377', u'aggregate_rating': u'4.4', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Embarcadero', u'city_id': 306, u'country_id': 216, u'zipcode': u'94111', u'longitude': u'-122.3934333333', u'address': u'Ferry Building, Level 1, 1 Ferry Plaza, Suite 11A, San Francisco 94111', u'latitude': u'37.7961000000', u'locality_verbose': u'Embarcadero, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/hog-island-oyster-company-embarcadero/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16844513}, u'price_range': 4, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Hog Island Oyster Company', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/hog-island-oyster-company-embarcadero?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Seafood, Chinese', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16849192_RESTAURANT_445996dd7e38959e819ab2778db17e2c_c.png', u'average_cost_for_two': 45, u'deeplink': u'zomato://restaurant/16849192', u'id': u'16849192', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16849192_RESTAURANT_445996dd7e38959e819ab2778db17e2c_c.png?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/r-g-lounge-chinatown/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/r-g-lounge-chinatown/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'685', u'aggregate_rating': u'4.2', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Chinatown', u'city_id': 306, u'country_id': 216, u'zipcode': u'94108', u'longitude': u'-122.4047694444', u'address': u'631 Kearny Street, San Francisco 94108', u'latitude': u'37.7939916667', u'locality_verbose': u'Chinatown, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/r-g-lounge-chinatown/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16849192}, u'price_range': 2, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'R &amp; G Lounge', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/r-g-lounge-chinatown?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'American, Desserts', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16841950_CHAIN_c88889c5b48823125e68b9562ad82d1d_c.png', u'average_cost_for_two': 40, u'deeplink': u'zomato://restaurant/16841952', u'id': u'16841952', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16841950_CHAIN_c88889c5b48823125e68b9562ad82d1d_c.png?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/the-cheesecake-factory-1-union-square/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/the-cheesecake-factory-1-union-square/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'272', u'aggregate_rating': u'4.0', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u"Macy's Marketplace", u'city_id': 306, u'country_id': 216, u'zipcode': u'94102', u'longitude': u'-122.4073900000', u'address': u"Macy's, Floor 8, 251 Geary Street, Union Square, San Francisco 94102", u'latitude': u'37.7873620000', u'locality_verbose': u"Macy's Marketplace, San Francisco"}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/the-cheesecake-factory-1-union-square/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16841952}, u'price_range': 2, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'The Cheesecake Factory', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/the-cheesecake-factory-1-union-square?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'California', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16849345_RESTAURANT_a910f88e6df9aed36643ef3b735b701a.png', u'average_cost_for_two': 210, u'deeplink': u'zomato://restaurant/16849345', u'id': u'16849345', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16849345_RESTAURANT_a910f88e6df9aed36643ef3b735b701a.png?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/gary-danko-fishermans-wharf/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/gary-danko-fishermans-wharf/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'765', u'aggregate_rating': u'4.4', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u"Fisherman's Wharf", u'city_id': 306, u'country_id': 216, u'zipcode': u'94109', u'longitude': u'-122.4205638889', u'address': u'800 North Point Street, San Francisco 94109', u'latitude': u'37.8057055556', u'locality_verbose': u"Fisherman's Wharf, San Francisco"}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/gary-danko-fishermans-wharf/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16849345}, u'price_range': 4, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Gary Danko', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/gary-danko-fishermans-wharf?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Seafood, American', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16851458_RESTAURANT_b37e70b80819a501e785b7a563cdcdff_c.jpg', u'average_cost_for_two': 80, u'deeplink': u'zomato://restaurant/16851458', u'id': u'16851458', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16851458_RESTAURANT_b37e70b80819a501e785b7a563cdcdff_c.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/tadich-grill-financial-district/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/tadich-grill-financial-district/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'825', u'aggregate_rating': u'4.4', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Financial District', u'city_id': 306, u'country_id': 216, u'zipcode': u'94111', u'longitude': u'-122.3993694444', u'address': u'240 California Street, San Francisco 94111', u'latitude': u'37.7931666667', u'locality_verbose': u'Financial District, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/tadich-grill-financial-district/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16851458}, u'price_range': 3, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Tadich Grill', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/tadich-grill-financial-district?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Italian', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16850754_RESTAURANT_43547ae7aee0aa463e373db169bf3029_c.jpg', u'average_cost_for_two': 75, u'deeplink': u'zomato://restaurant/16850754', u'id': u'16850754', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16850754_RESTAURANT_43547ae7aee0aa463e373db169bf3029_c.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/the-stinking-rose-north-beach/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/the-stinking-rose-north-beach/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'772', u'aggregate_rating': u'3.9', u'rating_text': u'Good', u'rating_color': u'9ACD32'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'North Beach', u'city_id': 306, u'country_id': 216, u'zipcode': u'94133', u'longitude': u'-122.4072638889', u'address': u'325 Columbus Avenue, San Francisco 94133', u'latitude': u'37.7981555556', u'locality_verbose': u'North Beach, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/the-stinking-rose-north-beach/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16850754}, u'price_range': 3, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'The Stinking Rose', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/the-stinking-rose-north-beach?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Bakery, Cafe', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16851686_RESTAURANT_800c26dde482eca93c3adcd23212c044_c.jpg', u'average_cost_for_two': 25, u'deeplink': u'zomato://restaurant/16851686', u'id': u'16851686', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16851686_RESTAURANT_800c26dde482eca93c3adcd23212c044_c.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/tartine-bakery-mission-district/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/tartine-bakery-mission-district/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'1354', u'aggregate_rating': u'4.9', u'rating_text': u'Excellent', u'rating_color': u'3F7E00'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Mission District', u'city_id': 306, u'country_id': 216, u'zipcode': u'94110', u'longitude': u'-122.4239500000', u'address': u'600 Guerrero Street, San Francisco 94110', u'latitude': u'37.7614861111', u'locality_verbose': u'Mission District, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/tartine-bakery-mission-district/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16851686}, u'price_range': 1, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Tartine Bakery', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/tartine-bakery-mission-district?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Burger, Fast Food', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16844845_CHAIN_c6a203688e8e293bac7fbd42dbd589c3_c.png', u'average_cost_for_two': 15, u'deeplink': u'zomato://restaurant/16844846', u'id': u'16844846', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16844845_CHAIN_c6a203688e8e293bac7fbd42dbd589c3_c.png?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/in-n-out-burger-fishermans-wharf/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/in-n-out-burger-fishermans-wharf/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'735', u'aggregate_rating': u'4.2', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u"Fisherman's Wharf", u'city_id': 306, u'country_id': 216, u'zipcode': u'94133', u'longitude': u'-122.4185777778', u'address': u'333 Jefferson Street, San Francisco 94133', u'latitude': u'37.8078472222', u'locality_verbose': u"Fisherman's Wharf, San Francisco"}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/in-n-out-burger-fishermans-wharf/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16844846}, u'price_range': 1, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'In-N-Out Burger', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/in-n-out-burger-fishermans-wharf?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Chinese', u'establishment_types': [], u'currency': u'$', u'featured_image': u'', u'average_cost_for_two': 0, u'deeplink': u'zomato://restaurant/16844677', u'id': u'16844677', u'switch_to_order_menu': 0, u'thumb': u'', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/house-of-nanking-chinatown/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/house-of-nanking-chinatown/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'938', u'aggregate_rating': u'4.3', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Chinatown', u'city_id': 306, u'country_id': 216, u'zipcode': u'94133', u'longitude': u'-122.4050916667', u'address': u'919 Kearny Street, San Francisco 94133', u'latitude': u'37.7964750000', u'locality_verbose': u'Chinatown, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/house-of-nanking-chinatown/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16844677}, u'price_range': 1, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'House of Nanking', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/house-of-nanking-chinatown?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Crepes, Sandwich, Burger', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16859330_RESTAURANT_5ca8a036daf6a65067bcb2bc184f681c_c.jpg', u'average_cost_for_two': 40, u'deeplink': u'zomato://restaurant/16859330', u'id': u'16859330', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16859330_RESTAURANT_5ca8a036daf6a65067bcb2bc184f681c_c.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/honey-honey-union-square/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/honey-honey-union-square/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'541', u'aggregate_rating': u'4.6', u'rating_text': u'Excellent', u'rating_color': u'3F7E00'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Union Square', u'city_id': 306, u'country_id': 216, u'zipcode': u'94102', u'longitude': u'-122.4115972222', u'address': u'599 Post Street, San Francisco 94102', u'latitude': u'37.7878944444', u'locality_verbose': u'Union Square, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/honey-honey-union-square/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16859330}, u'price_range': 2, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Honey Honey', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/honey-honey-union-square?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'California, Seafood', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16843658_RESTAURANT_d11dc180da7b11cb6682eb2a7fb2cb7a.png', u'average_cost_for_two': 120, u'deeplink': u'zomato://restaurant/16843658', u'id': u'16843658', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16843658_RESTAURANT_d11dc180da7b11cb6682eb2a7fb2cb7a.png?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/foreign-cinema-mission-district/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/foreign-cinema-mission-district/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'1129', u'aggregate_rating': u'4.5', u'rating_text': u'Excellent', u'rating_color': u'3F7E00'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Mission District', u'city_id': 306, u'country_id': 216, u'zipcode': u'94110', u'longitude': u'-122.4190444444', u'address': u'2534 Mission District Street, San Francisco 94110', u'latitude': u'37.7565305556', u'locality_verbose': u'Mission District, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/foreign-cinema-mission-district/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16843658}, u'price_range': 4, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Foreign Cinema', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/foreign-cinema-mission-district?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Italian', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16842751_RESTAURANT_f0c875da978db0b61e1ef5c974f2779c_c.jpg', u'average_cost_for_two': 55, u'deeplink': u'zomato://restaurant/16842751', u'id': u'16842751', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16842751_RESTAURANT_f0c875da978db0b61e1ef5c974f2779c_c.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/delfina-mission-district/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/delfina-mission-district/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'1492', u'aggregate_rating': u'4.8', u'rating_text': u'Excellent', u'rating_color': u'3F7E00'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Mission District', u'city_id': 306, u'country_id': 216, u'zipcode': u'94110', u'longitude': u'-122.4243694444', u'address': u'3621 18th Street, San Francisco 94110', u'latitude': u'37.7615388889', u'locality_verbose': u'Mission District, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/delfina-mission-district/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16842751}, u'price_range': 2, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Delfina', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/delfina-mission-district?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Vegetarian', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16844181_RESTAURANT_be312828371b3edc054a1890b24794bb_c.png?output-format=webp', u'average_cost_for_two': 50, u'deeplink': u'zomato://restaurant/16844181', u'id': u'16844181', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16844181_RESTAURANT_be312828371b3edc054a1890b24794bb_c.png?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/greens-marina-presidio/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/greens-marina-presidio/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'511', u'aggregate_rating': u'4.2', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Marina/Presidio', u'city_id': 306, u'country_id': 216, u'zipcode': u'94123', u'longitude': u'-122.4321444444', u'address': u'2 Marina Boulevard, San Francisco 94123', u'latitude': u'37.8067444444', u'locality_verbose': u'Marina/Presidio, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/greens-marina-presidio/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16844181}, u'price_range': 2, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Greens', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/greens-marina-presidio?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Italian, Seafood', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16849962_RESTAURANT_df96609dadf104beb31b3d0ed9202a54_c.jpg', u'average_cost_for_two': 85, u'deeplink': u'zomato://restaurant/16849962', u'id': u'16849962', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16849962_RESTAURANT_df96609dadf104beb31b3d0ed9202a54_c.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/scomas-fishermans-wharf/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/scomas-fishermans-wharf/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'1270', u'aggregate_rating': u'4.3', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u"Fisherman's Wharf", u'city_id': 306, u'country_id': 216, u'zipcode': u'94133', u'longitude': u'-122.4182500000', u'address': u'1965 Al Scoma Way, San Francisco 94133', u'latitude': u'37.8090527778', u'locality_verbose': u"Fisherman's Wharf, San Francisco"}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/scomas-fishermans-wharf/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16849962}, u'price_range': 3, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u"Scoma's", u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/scomas-fishermans-wharf?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Seafood, American', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16841078_RESTAURANT_7962db54e7c7ac1ecd7a254e9e37c013_c.jpg', u'average_cost_for_two': 65, u'deeplink': u'zomato://restaurant/16841078', u'id': u'16841078', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16841078_RESTAURANT_7962db54e7c7ac1ecd7a254e9e37c013_c.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/bubba-gump-shrimp-co-san-francisco/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/bubba-gump-shrimp-co-san-francisco/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'286', u'aggregate_rating': u'4.1', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u"Fisherman's Wharf", u'city_id': 306, u'country_id': 216, u'zipcode': u'94133', u'longitude': u'-122.4104305556', u'address': u'Pier 39, San Francisco 94133', u'latitude': u'37.8109694444', u'locality_verbose': u"Fisherman's Wharf, San Francisco"}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/bubba-gump-shrimp-co-san-francisco/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16841078}, u'price_range': 3, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Bubba Gump Shrimp Co.', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/bubba-gump-shrimp-co-san-francisco?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'California, Fusion', u'establishment_types': [], u'currency': u'$', u'featured_image': u'', u'average_cost_for_two': 80, u'deeplink': u'zomato://restaurant/16860927', u'id': u'16860927', u'switch_to_order_menu': 0, u'thumb': u'', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/state-bird-provisions-western-addition/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/state-bird-provisions-western-addition/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'572', u'aggregate_rating': u'4.4', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Western Addition', u'city_id': 306, u'country_id': 216, u'zipcode': u'94115', u'longitude': u'-122.4329481000', u'address': u'1529 Fillmore Street, San Francisco 94115', u'latitude': u'37.7837361000', u'locality_verbose': u'Western Addition, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/state-bird-provisions-western-addition/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16860927}, u'price_range': 3, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'State Bird Provisions', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/state-bird-provisions-western-addition?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Ice Cream', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16852987_RESTAURANT_82f3f22d2f8af45d3001cd2e5f82e6aa_c.jpg', u'average_cost_for_two': 15, u'deeplink': u'zomato://restaurant/16852987', u'id': u'16852987', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16852987_RESTAURANT_82f3f22d2f8af45d3001cd2e5f82e6aa_c.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/bi-rite-creamery-bakeshop-mission-district/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/bi-rite-creamery-bakeshop-mission-district/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'541', u'aggregate_rating': u'4.7', u'rating_text': u'Excellent', u'rating_color': u'3F7E00'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Mission District', u'city_id': 306, u'country_id': 216, u'zipcode': u'94110', u'longitude': u'-122.4257055556', u'address': u'3692 18th Street, San Francisco 94110', u'latitude': u'37.7614833333', u'locality_verbose': u'Mission District, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/bi-rite-creamery-bakeshop-mission-district/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16852987}, u'price_range': 1, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Bi-Rite Creamery &amp; Bakeshop', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/bi-rite-creamery-bakeshop-mission-district?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Pizza, Italian', u'establishment_types': [], u'currency': u'$', u'featured_image': u'', u'average_cost_for_two': 35, u'deeplink': u'zomato://restaurant/16852308', u'id': u'16852308', u'switch_to_order_menu': 0, u'thumb': u'', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/uncle-vitos-pizzeria-nob-hill/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/uncle-vitos-pizzeria-nob-hill/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'392', u'aggregate_rating': u'4.3', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Nob Hill', u'city_id': 306, u'country_id': 216, u'zipcode': u'94108', u'longitude': u'-122.4087972222', u'address': u'700 Bush Street, San Francisco 94108', u'latitude': u'37.7901416667', u'locality_verbose': u'Nob Hill, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/uncle-vitos-pizzeria-nob-hill/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16852308}, u'price_range': 2, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u"Uncle Vito's Pizzeria", u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/uncle-vitos-pizzeria-nob-hill?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'American, French', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16840989_RESTAURANT_3b4ea2279743f39b0a1222a9bb95ad81_c.jpg', u'average_cost_for_two': 120, u'deeplink': u'zomato://restaurant/16840989', u'id': u'16840989', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16840989_RESTAURANT_3b4ea2279743f39b0a1222a9bb95ad81_c.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/boulevard-embarcadero/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/boulevard-embarcadero/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'808', u'aggregate_rating': u'4.4', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Embarcadero', u'city_id': 306, u'country_id': 216, u'zipcode': u'94105', u'longitude': u'-122.3927820000', u'address': u'1 Mission Street, San Francisco 94105', u'latitude': u'37.7935660000', u'locality_verbose': u'Embarcadero, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/boulevard-embarcadero/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16840989}, u'price_range': 4, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Boulevard', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/boulevard-embarcadero?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'American', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16846718_RESTAURANT_a7931f37bee20b003fe11e702a5a9106_c.jpg', u'average_cost_for_two': 40, u'deeplink': u'zomato://restaurant/16846718', u'id': u'16846718', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16846718_RESTAURANT_a7931f37bee20b003fe11e702a5a9106_c.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/mamas-on-washington-square-north-beach/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/mamas-on-washington-square-north-beach/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'444', u'aggregate_rating': u'4.4', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'North Beach', u'city_id': 306, u'country_id': 216, u'zipcode': u'94133', u'longitude': u'-122.4094777778', u'address': u'1701 Stockton Street, San Francisco 94133', u'latitude': u'37.8013833333', u'locality_verbose': u'North Beach, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/mamas-on-washington-square-north-beach/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16846718}, u'price_range': 2, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u"Mama's on Washington Square", u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/mamas-on-washington-square-north-beach?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Seafood', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16848732_RESTAURANT_96834dcc322987ea3336aaf706c6e704_c.jpg', u'average_cost_for_two': 55, u'deeplink': u'zomato://restaurant/16848732', u'id': u'16848732', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16848732_RESTAURANT_96834dcc322987ea3336aaf706c6e704_c.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/pier-market-fishermans-wharf/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/pier-market-fishermans-wharf/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'229', u'aggregate_rating': u'4.0', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u"Fisherman's Wharf", u'city_id': 306, u'country_id': 216, u'zipcode': u'94133', u'longitude': u'-122.4104527778', u'address': u'Pier 39, San Francisco 94133', u'latitude': u'37.8099833333', u'locality_verbose': u"Fisherman's Wharf, San Francisco"}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/pier-market-fishermans-wharf/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16848732}, u'price_range': 2, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Pier Market', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/pier-market-fishermans-wharf?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Burger, American', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16851726_RESTAURANT_1ae3d95632853f0958d6259999578366_c.jpg', u'average_cost_for_two': 50, u'deeplink': u'zomato://restaurant/16851726', u'id': u'16851726', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16851726_RESTAURANT_1ae3d95632853f0958d6259999578366_c.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/gotts-roadside-embarcadero/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/gotts-roadside-embarcadero/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'258', u'aggregate_rating': u'4.0', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Ferry Building ', u'city_id': 306, u'country_id': 216, u'zipcode': u'94111', u'longitude': u'-122.3942805556', u'address': u'Ferry Building, Level 1, 1 Ferry Plaza, Suite 6, San Francisco 94111', u'latitude': u'37.7959222222', u'locality_verbose': u'Ferry Building , San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/gotts-roadside-embarcadero/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16851726}, u'price_range': 2, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u"Gott's Roadside", u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/gotts-roadside-embarcadero?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Cafe, Bakery', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16840979_RESTAURANT_46f284d0c296bb475bd55d2c03681904.png', u'average_cost_for_two': 25, u'deeplink': u'zomato://restaurant/16840979', u'id': u'16840979', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16840979_RESTAURANT_46f284d0c296bb475bd55d2c03681904.png?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/boudin-bakery-cafe-fishermans-wharf/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/boudin-bakery-cafe-fishermans-wharf/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'218', u'aggregate_rating': u'4.3', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u"Fisherman's Wharf", u'city_id': 306, u'country_id': 216, u'zipcode': u'94133', u'longitude': u'-122.4100027778', u'address': u'Pier 39, San Francisco 94133', u'latitude': u'37.8088722222', u'locality_verbose': u"Fisherman's Wharf, San Francisco"}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/boudin-bakery-cafe-fishermans-wharf/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16840979}, u'price_range': 1, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Boudin Bakery &amp; Cafe', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/boudin-bakery-cafe-fishermans-wharf?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'American', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16842986_RESTAURANT_59cdcda3f40d90adaa81cef9015d49a5_c.jpg', u'average_cost_for_two': 50, u'deeplink': u'zomato://restaurant/16842986', u'id': u'16842986', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16842986_RESTAURANT_59cdcda3f40d90adaa81cef9015d49a5_c.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/dotties-soma/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/dotties-soma/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'661', u'aggregate_rating': u'4.4', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'SOMA', u'city_id': 306, u'country_id': 216, u'zipcode': u'94103', u'longitude': u'-122.4098361111', u'address': u'28 6th Street, San Francisco 94103', u'latitude': u'37.7817527778', u'locality_verbose': u'SOMA, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/dotties-soma/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16842986}, u'price_range': 2, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u"Dottie's", u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/dotties-soma?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'California, Italian, Pizza', u'establishment_types': [], u'currency': u'$', u'featured_image': u'', u'average_cost_for_two': 65, u'deeplink': u'zomato://restaurant/16858164', u'id': u'16858164', u'switch_to_order_menu': 0, u'thumb': u'', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/flour-water-mission-district/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/flour-water-mission-district/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'335', u'aggregate_rating': u'4.0', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Mission District', u'city_id': 306, u'country_id': 216, u'zipcode': u'94110', u'longitude': u'-122.4124611111', u'address': u'2401 Harrison Street, San Francisco 94110', u'latitude': u'37.7589333333', u'locality_verbose': u'Mission District, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/flour-water-mission-district/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16858164}, u'price_range': 3, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Flour + Water', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/flour-water-mission-district?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'French', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16841519_RESTAURANT_be632803838303e5499e72265daaf028.jpg', u'average_cost_for_two': 80, u'deeplink': u'zomato://restaurant/16841519', u'id': u'16841519', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16841519_RESTAURANT_be632803838303e5499e72265daaf028.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/cafe-de-la-presse-union-square/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/cafe-de-la-presse-union-square/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'275', u'aggregate_rating': u'4.0', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Union Square', u'city_id': 306, u'country_id': 216, u'zipcode': u'94108', u'longitude': u'-122.4056861111', u'address': u'352 Grant Avenue, San Francisco 94108', u'latitude': u'37.7905472222', u'locality_verbose': u'Union Square, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/cafe-de-la-presse-union-square/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16841519}, u'price_range': 3, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Cafe De La Presse', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/cafe-de-la-presse-union-square?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Steak', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16844681_RESTAURANT_555c28a4ba50c86a3f61e50dea73cc29.jpg?output-format=webp', u'average_cost_for_two': 110, u'deeplink': u'zomato://restaurant/16844681', u'id': u'16844681', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16844681_RESTAURANT_555c28a4ba50c86a3f61e50dea73cc29.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/house-of-prime-rib-nob-hill/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/house-of-prime-rib-nob-hill/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'588', u'aggregate_rating': u'4.5', u'rating_text': u'Excellent', u'rating_color': u'3F7E00'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Nob Hill', u'city_id': 306, u'country_id': 216, u'zipcode': u'94109', u'longitude': u'-122.4230277778', u'address': u'1906 Van Ness Avenue,  San Francisco 94109', u'latitude': u'37.7932916667', u'locality_verbose': u'Nob Hill, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/house-of-prime-rib-nob-hill/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16844681}, u'price_range': 4, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'House Of Prime Rib', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/house-of-prime-rib-nob-hill?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Cuban, Tapas, Caribbean', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16841875_RESTAURANT_2d0e0d55d50ba29c5d5efdbe485d1f49_c.jpg', u'average_cost_for_two': 50, u'deeplink': u'zomato://restaurant/16841875', u'id': u'16841875', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16841875_RESTAURANT_2d0e0d55d50ba29c5d5efdbe485d1f49_c.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/cha-cha-cha-haight/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/cha-cha-cha-haight/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'832', u'aggregate_rating': u'4.4', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Haight', u'city_id': 306, u'country_id': 216, u'zipcode': u'94117', u'longitude': u'-122.4519277778', u'address': u'1801 Haight Street, San Francisco 94117', u'latitude': u'37.7692527778', u'locality_verbose': u'Haight, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/cha-cha-cha-haight/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16841875}, u'price_range': 2, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Cha Cha Cha', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/cha-cha-cha-haight?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Burmese', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16841211_CHAIN_342998827ea9e956c1a1f284dac143af.png', u'average_cost_for_two': 50, u'deeplink': u'zomato://restaurant/16841211', u'id': u'16841211', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16841211_CHAIN_342998827ea9e956c1a1f284dac143af.png?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/burma-superstar-inner-richmond/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/burma-superstar-inner-richmond/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'843', u'aggregate_rating': u'4.7', u'rating_text': u'Excellent', u'rating_color': u'3F7E00'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Inner Richmond', u'city_id': 306, u'country_id': 216, u'zipcode': u'94118', u'longitude': u'-122.4625472222', u'address': u'309 Clement Street, San Francisco 94118', u'latitude': u'37.7830361111', u'locality_verbose': u'Inner Richmond, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/burma-superstar-inner-richmond/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16841211}, u'price_range': 2, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Burma Superstar', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/burma-superstar-inner-richmond?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Ice Cream', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16857688_RESTAURANT_d3469ae212236040505f06165b81a93c_c.JPG', u'average_cost_for_two': 10, u'deeplink': u'zomato://restaurant/16857688', u'id': u'16857688', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16857688_RESTAURANT_d3469ae212236040505f06165b81a93c_c.JPG?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/humphry-slocombe-mission-district/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/humphry-slocombe-mission-district/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'364', u'aggregate_rating': u'4.4', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Mission District', u'city_id': 306, u'country_id': 216, u'zipcode': u'94110', u'longitude': u'-122.4118950000', u'address': u'2790 A Harrison Street, San Francisco 94110', u'latitude': u'37.7527680000', u'locality_verbose': u'Mission District, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/humphry-slocombe-mission-district/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16857688}, u'price_range': 1, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Humphry Slocombe', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/humphry-slocombe-mission-district?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Seafood', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16852997_RESTAURANT_d84af2c8001564205fcefc8a00a63504_c.jpg', u'average_cost_for_two': 100, u'deeplink': u'zomato://restaurant/16852997', u'id': u'16852997', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16852997_RESTAURANT_d84af2c8001564205fcefc8a00a63504_c.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/fog-harbor-fish-house-fishermans-wharf/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/fog-harbor-fish-house-fishermans-wharf/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'551', u'aggregate_rating': u'4.4', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u"Fisherman's Wharf", u'city_id': 306, u'country_id': 216, u'zipcode': u'94133', u'longitude': u'-122.4102083333', u'address': u'Pier 39, Suite 202, San Francisco 94133', u'latitude': u'37.8088500000', u'locality_verbose': u"Fisherman's Wharf, San Francisco"}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/fog-harbor-fish-house-fishermans-wharf/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16852997}, u'price_range': 4, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Fog Harbor Fish House', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/fog-harbor-fish-house-fishermans-wharf?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Seafood', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16860402_RESTAURANT_56cd1405b2db99173c74b24c7bc78262_c.jpg', u'average_cost_for_two': 25, u'deeplink': u'zomato://restaurant/16860402', u'id': u'16860402', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16860402_RESTAURANT_56cd1405b2db99173c74b24c7bc78262_c.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/the-codmother-fish-and-chips-fishermans-wharf/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/the-codmother-fish-and-chips-fishermans-wharf/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'165', u'aggregate_rating': u'4.1', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u"Fisherman's Wharf", u'city_id': 306, u'country_id': 216, u'zipcode': u'94133', u'longitude': u'-122.4172361111', u'address': u'496 Beach Street, San Francisco 94133', u'latitude': u'37.8073222222', u'locality_verbose': u"Fisherman's Wharf, San Francisco"}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/the-codmother-fish-and-chips-fishermans-wharf/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16860402}, u'price_range': 1, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'The Codmother Fish and Chips', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/the-codmother-fish-and-chips-fishermans-wharf?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Greek, Mediterranean', u'establishment_types': [], u'currency': u'$', u'featured_image': u'', u'average_cost_for_two': 100, u'deeplink': u'zomato://restaurant/16845743', u'id': u'16845743', u'switch_to_order_menu': 0, u'thumb': u'', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/kokkari-estiatorio-financial-district/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/kokkari-estiatorio-financial-district/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'547', u'aggregate_rating': u'4.5', u'rating_text': u'Excellent', u'rating_color': u'3F7E00'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Financial District', u'city_id': 306, u'country_id': 216, u'zipcode': u'94111', u'longitude': u'-122.3994055556', u'address': u'200 Jackson Street, San Francisco 94111', u'latitude': u'37.7970277778', u'locality_verbose': u'Financial District, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/kokkari-estiatorio-financial-district/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16845743}, u'price_range': 4, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Kokkari Estiatorio', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/kokkari-estiatorio-financial-district?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'American, California', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16842179_RESTAURANT_83255713a0e94901ae9f516db2142f73.jpg', u'average_cost_for_two': 45, u'deeplink': u'zomato://restaurant/16842179', u'id': u'16842179', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16842179_RESTAURANT_83255713a0e94901ae9f516db2142f73.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/chow-castro/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/chow-castro/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'893', u'aggregate_rating': u'4.4', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Castro', u'city_id': 306, u'country_id': 216, u'zipcode': u'94114', u'longitude': u'-122.4290166667', u'address': u'215 Church Street, San Francisco 94114', u'latitude': u'37.7671472222', u'locality_verbose': u'Castro, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/chow-castro/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16842179}, u'price_range': 2, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Chow', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/chow-castro?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'California', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16847879_RESTAURANT_22344f4858fd9e0489c40d9daf0e34e6.jpg', u'average_cost_for_two': 100, u'deeplink': u'zomato://restaurant/16847879', u'id': u'16847879', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16847879_RESTAURANT_22344f4858fd9e0489c40d9daf0e34e6.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/nopa-western-addition/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/nopa-western-addition/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'635', u'aggregate_rating': u'4.5', u'rating_text': u'Excellent', u'rating_color': u'3F7E00'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Western Addition', u'city_id': 306, u'country_id': 216, u'zipcode': u'94117', u'longitude': u'-122.4378805556', u'address': u'560 Divisadero Street, San Francisco 94117', u'latitude': u'37.7748527778', u'locality_verbose': u'Western Addition, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/nopa-western-addition/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16847879}, u'price_range': 4, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Nopa', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/nopa-western-addition?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Seafood', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16843703_RESTAURANT_b7642d08c9677bd3650bdd0ef6de2bbd.jpg', u'average_cost_for_two': 65, u'deeplink': u'zomato://restaurant/16843703', u'id': u'16843703', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16843703_RESTAURANT_b7642d08c9677bd3650bdd0ef6de2bbd.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/franciscan-crab-san-francisco/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/franciscan-crab-san-francisco/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'310', u'aggregate_rating': u'4.1', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u"Fisherman's Wharf", u'city_id': 306, u'country_id': 216, u'zipcode': u'94133', u'longitude': u'-122.4147500000', u'address': u'Pier 43, San Francisco 94133', u'latitude': u'37.8092027778', u'locality_verbose': u"Fisherman's Wharf, San Francisco"}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/franciscan-crab-san-francisco/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16843703}, u'price_range': 3, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Franciscan Crab', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/franciscan-crab-san-francisco?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'German', u'establishment_types': [], u'currency': u'$', u'featured_image': u'', u'average_cost_for_two': 43, u'deeplink': u'zomato://restaurant/16851090', u'id': u'16851090', u'switch_to_order_menu': 0, u'thumb': u'', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/suppenk\xfcche-western-addition/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/suppenk\xfcche-western-addition/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'822', u'aggregate_rating': u'4.6', u'rating_text': u'Excellent', u'rating_color': u'3F7E00'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Western Addition', u'city_id': 306, u'country_id': 216, u'zipcode': u'94102', u'longitude': u'-122.4262720000', u'address': u'525 Laguna Street, San Francisco 94102', u'latitude': u'37.7760850000', u'locality_verbose': u'Western Addition, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/suppenk\xfcche-western-addition/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16851090}, u'price_range': 2, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Suppenk\xfcche', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/suppenk\xfcche-western-addition?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'American', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16857729_RESTAURANT_9a160760c3e3cf5674fc147af8d27ed0_c.jpg', u'average_cost_for_two': 50, u'deeplink': u'zomato://restaurant/16857729', u'id': u'16857729', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16857729_RESTAURANT_9a160760c3e3cf5674fc147af8d27ed0_c.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/the-buena-vista-fishermans-wharf/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/the-buena-vista-fishermans-wharf/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'442', u'aggregate_rating': u'4.2', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u"Fisherman's Wharf", u'city_id': 306, u'country_id': 216, u'zipcode': u'94109', u'longitude': u'-122.4206611111', u'address': u'2765 Hyde Street, San Francisco 94109', u'latitude': u'37.8066250000', u'locality_verbose': u"Fisherman's Wharf, San Francisco"}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/the-buena-vista-fishermans-wharf/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16857729}, u'price_range': 2, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'The Buena Vista', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/the-buena-vista-fishermans-wharf?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Chinese', u'establishment_types': [], u'currency': u'$', u'featured_image': u'', u'average_cost_for_two': 40, u'deeplink': u'zomato://restaurant/16852772', u'id': u'16852772', u'switch_to_order_menu': 0, u'thumb': u'', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/yank-sing-2-go-soma/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/yank-sing-2-go-soma/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'573', u'aggregate_rating': u'4.3', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Rincon Center', u'city_id': 306, u'country_id': 216, u'zipcode': u'94105', u'longitude': u'-122.3938280000', u'address': u'Rincon Center, 101 Spear Street, San Francisco 94105', u'latitude': u'37.7925690000', u'locality_verbose': u'Rincon Center, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/yank-sing-2-go-soma/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16852772}, u'price_range': 2, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Yank Sing 2 Go', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/yank-sing-2-go-soma?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Diner', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16851725_RESTAURANT_38967c6e85d952169bd7b5d1a455f49b_c.jpg', u'average_cost_for_two': 30, u'deeplink': u'zomato://restaurant/16851725', u'id': u'16851725', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16851725_RESTAURANT_38967c6e85d952169bd7b5d1a455f49b_c.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/taylor-street-coffee-shop-civic-center/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/taylor-street-coffee-shop-civic-center/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'247', u'aggregate_rating': u'4.4', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Civic Center', u'city_id': 306, u'country_id': 216, u'zipcode': u'94102', u'longitude': u'-122.4109638889', u'address': u'375 Taylor Street, San Francisco 94102', u'latitude': u'37.7858388889', u'locality_verbose': u'Civic Center, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/taylor-street-coffee-shop-civic-center/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16851725}, u'price_range': 2, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Taylor Street Coffee Shop', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/taylor-street-coffee-shop-civic-center?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'American', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16849987_RESTAURANT_8cf032b7e3fc4bd52bdff5d4382d8bc7_c.JPG', u'average_cost_for_two': 75, u'deeplink': u'zomato://restaurant/16849987', u'id': u'16849987', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16849987_RESTAURANT_8cf032b7e3fc4bd52bdff5d4382d8bc7_c.JPG?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/sears-fine-food-union-square/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/sears-fine-food-union-square/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'449', u'aggregate_rating': u'4.0', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Union Square', u'city_id': 306, u'country_id': 216, u'zipcode': u'94102', u'longitude': u'-122.4083638889', u'address': u'439 Powell Street, San Francisco 94102', u'latitude': u'37.7888416667', u'locality_verbose': u'Union Square, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/sears-fine-food-union-square/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16849987}, u'price_range': 3, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Sears Fine Food', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/sears-fine-food-union-square?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'French, American', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16839883_RESTAURANT_fddf0f3910836612d677927b4861c5a8.png?output-format=webp', u'average_cost_for_two': 70, u'deeplink': u'zomato://restaurant/16839883', u'id': u'16839883', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16839883_RESTAURANT_fddf0f3910836612d677927b4861c5a8.png?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/absinthe-civic-center/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/absinthe-civic-center/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'509', u'aggregate_rating': u'4.2', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Civic Center', u'city_id': 306, u'country_id': 216, u'zipcode': u'94102', u'longitude': u'-122.4229277778', u'address': u'398 Hayes Street, San Francisco 94102', u'latitude': u'37.7769916667', u'locality_verbose': u'Civic Center, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/absinthe-civic-center/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16839883}, u'price_range': 3, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Absinthe', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/absinthe-civic-center?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Mexican', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16846029_RESTAURANT_2157d7ff145dfb3aa8250bb9db72b45a_c.png', u'average_cost_for_two': 25, u'deeplink': u'zomato://restaurant/16846029', u'id': u'16846029', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16846029_RESTAURANT_2157d7ff145dfb3aa8250bb9db72b45a_c.png?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/la-taqueria-mission-district/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/la-taqueria-mission-district/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'483', u'aggregate_rating': u'4.3', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Mission District', u'city_id': 306, u'country_id': 216, u'zipcode': u'94110', u'longitude': u'-122.4182277778', u'address': u'2889 Mission District Street, San Francisco 94110', u'latitude': u'37.7508722222', u'locality_verbose': u'Mission District, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/la-taqueria-mission-district/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16846029}, u'price_range': 1, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'La Taqueria', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/la-taqueria-mission-district?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Italian, Pizza', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16839872_RESTAURANT_da47de5892c3034d970bbfd2b5d5b2de.jpg', u'average_cost_for_two': 75, u'deeplink': u'zomato://restaurant/16839872', u'id': u'16839872', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16839872_RESTAURANT_da47de5892c3034d970bbfd2b5d5b2de.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/a16-marina-presidio/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/a16-marina-presidio/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'535', u'aggregate_rating': u'4.0', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Marina/Presidio', u'city_id': 306, u'country_id': 216, u'zipcode': u'94123', u'longitude': u'-122.4421611111', u'address': u'2355 Chestnut Street, San Francisco 94123', u'latitude': u'37.8000444444', u'locality_verbose': u'Marina/Presidio, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/a16-marina-presidio/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16839872}, u'price_range': 3, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'A16', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/a16-marina-presidio?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'French, Seafood', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16848900_RESTAURANT_58e75df20bb276a98136c874af2c89dd.jpg', u'average_cost_for_two': 50, u'deeplink': u'zomato://restaurant/16848900', u'id': u'16848900', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16848900_RESTAURANT_58e75df20bb276a98136c874af2c89dd.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/plouf-financial-district/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/plouf-financial-district/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'151', u'aggregate_rating': u'3.7', u'rating_text': u'Good', u'rating_color': u'9ACD32'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Financial District', u'city_id': 306, u'country_id': 216, u'zipcode': u'94104', u'longitude': u'-122.4032527778', u'address': u'40 Belden Place, San Francisco 94104', u'latitude': u'37.7913694444', u'locality_verbose': u'Financial District, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/plouf-financial-district/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16848900}, u'price_range': 2, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Plouf', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/plouf-financial-district?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Burger, American', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16859449_RESTAURANT_05a34ec1613352d47debbcef0e2f53d9.png', u'average_cost_for_two': 75, u'deeplink': u'zomato://restaurant/16859449', u'id': u'16859449', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16859449_RESTAURANT_05a34ec1613352d47debbcef0e2f53d9.png?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/wayfare-tavern-financial-district/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/wayfare-tavern-financial-district/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'356', u'aggregate_rating': u'4.3', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Financial District', u'city_id': 306, u'country_id': 216, u'zipcode': u'94111', u'longitude': u'-122.4023055556', u'address': u'558 Sacramento Street, San Francisco 94111', u'latitude': u'37.7938694444', u'locality_verbose': u'Financial District, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/wayfare-tavern-financial-district/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16859449}, u'price_range': 3, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Wayfare Tavern', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/wayfare-tavern-financial-district?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'American, Breakfast', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16859172_RESTAURANT_744da7dc4f6d414dc750c62bb6e4ec63_c.jpg', u'average_cost_for_two': 40, u'deeplink': u'zomato://restaurant/16859172', u'id': u'16859172', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16859172_RESTAURANT_744da7dc4f6d414dc750c62bb6e4ec63_c.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/the-grove-yerba-buena-soma/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/the-grove-yerba-buena-soma/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'274', u'aggregate_rating': u'4.3', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'SOMA', u'city_id': 306, u'country_id': 216, u'zipcode': u'94105', u'longitude': u'-122.4018555556', u'address': u'690 Mission Street, San Francisco 94105', u'latitude': u'37.7864138889', u'locality_verbose': u'SOMA, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/the-grove-yerba-buena-soma/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16859172}, u'price_range': 2, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'The Grove Yerba Buena', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/the-grove-yerba-buena-soma?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'American, Seafood, Bakery', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16840810_RESTAURANT_0b6ae150742c945a4e56dfee5e7f6baa.jpg', u'average_cost_for_two': 70, u'deeplink': u'zomato://restaurant/16840810', u'id': u'16840810', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16840810_RESTAURANT_0b6ae150742c945a4e56dfee5e7f6baa.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/bistro-boudin-fishermans-wharf/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/bistro-boudin-fishermans-wharf/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'334', u'aggregate_rating': u'4.0', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u"Fisherman's Wharf", u'city_id': 306, u'country_id': 216, u'zipcode': u'94133', u'longitude': u'-122.4150166667', u'address': u'160 Jefferson Street, San Francisco 94133', u'latitude': u'37.8084916667', u'locality_verbose': u"Fisherman's Wharf, San Francisco"}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/bistro-boudin-fishermans-wharf/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16840810}, u'price_range': 3, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Bistro Boudin', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/bistro-boudin-fishermans-wharf?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Seafood, Italian', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16839995_RESTAURANT_76f29a6078d1712733899e0b85801099_c.jpg', u'average_cost_for_two': 55, u'deeplink': u'zomato://restaurant/16839995', u'id': u'16839995', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16839995_RESTAURANT_76f29a6078d1712733899e0b85801099_c.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/aliotos-fish-co-ltd-fishermans-wharf/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/aliotos-fish-co-ltd-fishermans-wharf/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'386', u'aggregate_rating': u'3.8', u'rating_text': u'Good', u'rating_color': u'9ACD32'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u"Fisherman's Wharf", u'city_id': 306, u'country_id': 216, u'zipcode': u'94133', u'longitude': u'-122.4185420000', u'address': u'360 Jefferson Street, San Francisco 94133', u'latitude': u'37.8080190000', u'locality_verbose': u"Fisherman's Wharf, San Francisco"}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/aliotos-fish-co-ltd-fishermans-wharf/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16839995}, u'price_range': 2, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u"Alioto's Fish Co Ltd", u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/aliotos-fish-co-ltd-fishermans-wharf?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Coffee and Tea', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16859109_CHAIN_e771756ca9607a718a6d5d6e081aa40e_c.png', u'average_cost_for_two': 15, u'deeplink': u'zomato://restaurant/16859109', u'id': u'16859109', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16859109_CHAIN_e771756ca9607a718a6d5d6e081aa40e_c.png?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/blue-bottle-coffee-embarcadero/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/blue-bottle-coffee-embarcadero/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'132', u'aggregate_rating': u'3.9', u'rating_text': u'Good', u'rating_color': u'9ACD32'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Ferry Building ', u'city_id': 306, u'country_id': 216, u'zipcode': u'94111', u'longitude': u'-122.3938833333', u'address': u'Ferry Building, Level 1, 1 Ferry Plaza, Suite 7, San Francisco 94111', u'latitude': u'37.7959166667', u'locality_verbose': u'Ferry Building , San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/blue-bottle-coffee-embarcadero/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16859109}, u'price_range': 1, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Blue Bottle', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/blue-bottle-coffee-embarcadero?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Seafood', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16851232_RESTAURANT_583041de1e29306fc01f65185af715ad_c.jpg', u'average_cost_for_two': 40, u'deeplink': u'zomato://restaurant/16851232', u'id': u'16851232', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16851232_RESTAURANT_583041de1e29306fc01f65185af715ad_c.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/swan-oyster-depot-nob-hill/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/swan-oyster-depot-nob-hill/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'417', u'aggregate_rating': u'4.3', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Nob Hill', u'city_id': 306, u'country_id': 216, u'zipcode': u'94109', u'longitude': u'-122.4209230000', u'address': u'1517 Polk Street, San Francisco 94109', u'latitude': u'37.7908210000', u'locality_verbose': u'Nob Hill, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/swan-oyster-depot-nob-hill/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16851232}, u'price_range': 2, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Swan Oyster Depot', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/swan-oyster-depot-nob-hill?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Indian, California', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16842985_RESTAURANT_fb02544926111a2b4ce74aaefd39db26.png', u'average_cost_for_two': 85, u'deeplink': u'zomato://restaurant/16842985', u'id': u'16842985', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16842985_RESTAURANT_fb02544926111a2b4ce74aaefd39db26.png?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/dosa-mission-district/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/dosa-mission-district/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'430', u'aggregate_rating': u'4.2', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Mission District', u'city_id': 306, u'country_id': 216, u'zipcode': u'94110', u'longitude': u'-122.4213166667', u'address': u'995 Valencia Street, San Francisco 94110', u'latitude': u'37.7571527778', u'locality_verbose': u'Mission District, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/dosa-mission-district/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16842985}, u'price_range': 3, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Dosa', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/dosa-mission-district?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'American', u'establishment_types': [], u'currency': u'$', u'featured_image': u'', u'average_cost_for_two': 30, u'deeplink': u'zomato://restaurant/16841416', u'id': u'16841416', u'switch_to_order_menu': 0, u'thumb': u'', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/cafe-mason-union-square/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/cafe-mason-union-square/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'183', u'aggregate_rating': u'3.7', u'rating_text': u'Good', u'rating_color': u'9ACD32'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Union Square', u'city_id': 306, u'country_id': 216, u'zipcode': u'94102', u'longitude': u'-122.4097750000', u'address': u'312 Mason Street, San Francisco 94102', u'latitude': u'37.7866333333', u'locality_verbose': u'Union Square, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/cafe-mason-union-square/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16841416}, u'price_range': 2, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Cafe Mason', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/cafe-mason-union-square?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'American', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16844384_RESTAURANT_028b35a09e7ee53691f5b05a2dbad6da_c.jpg', u'average_cost_for_two': 55, u'deeplink': u'zomato://restaurant/16844384', u'id': u'16844384', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16844384_RESTAURANT_028b35a09e7ee53691f5b05a2dbad6da_c.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/hard-rock-cafe-fishermans-wharf/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/hard-rock-cafe-fishermans-wharf/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'104', u'aggregate_rating': u'3.5', u'rating_text': u'Good', u'rating_color': u'9ACD32'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u"Fisherman's Wharf", u'city_id': 306, u'country_id': 216, u'zipcode': u'94133', u'longitude': u'-122.4099194444', u'address': u'Pier 39, San Francisco 94133', u'latitude': u'37.8086305556', u'locality_verbose': u"Fisherman's Wharf, San Francisco"}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/hard-rock-cafe-fishermans-wharf/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16844384}, u'price_range': 2, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Hard Rock Cafe', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/hard-rock-cafe-fishermans-wharf?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Seafood', u'establishment_types': [], u'currency': u'$', u'featured_image': u'', u'average_cost_for_two': 60, u'deeplink': u'zomato://restaurant/16842517', u'id': u'16842517', u'switch_to_order_menu': 0, u'thumb': u'', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/crab-house-fishermans-wharf/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/crab-house-fishermans-wharf/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'218', u'aggregate_rating': u'3.9', u'rating_text': u'Good', u'rating_color': u'9ACD32'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u"Fisherman's Wharf", u'city_id': 306, u'country_id': 216, u'zipcode': u'94133', u'longitude': u'-122.4103472222', u'address': u'203 Pier 39, San Francisco 94133', u'latitude': u'37.8094972222', u'locality_verbose': u"Fisherman's Wharf, San Francisco"}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/crab-house-fishermans-wharf/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16842517}, u'price_range': 3, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Crab House', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/crab-house-fishermans-wharf?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'American, Burger', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16858698_RESTAURANT_8231ad3c1a06570fddc32b6ef56a0257_c.jpg', u'average_cost_for_two': 30, u'deeplink': u'zomato://restaurant/16858698', u'id': u'16858698', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16858698_RESTAURANT_8231ad3c1a06570fddc32b6ef56a0257_c.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/hollywood-cafe-fishermans-wharf/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/hollywood-cafe-fishermans-wharf/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'339', u'aggregate_rating': u'4.6', u'rating_text': u'Excellent', u'rating_color': u'3F7E00'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u"Fisherman's Wharf", u'city_id': 306, u'country_id': 216, u'zipcode': u'94133', u'longitude': u'-122.4158250000', u'address': u'530 North Point Street, San Francisco 94133', u'latitude': u'37.8063472222', u'locality_verbose': u"Fisherman's Wharf, San Francisco"}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/hollywood-cafe-fishermans-wharf/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16858698}, u'price_range': 2, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Hollywood Cafe', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/hollywood-cafe-fishermans-wharf?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Dim Sum, Chinese', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16852773_RESTAURANT_727ca2cc350b07299d7b086932c9d97b_c.jpg', u'average_cost_for_two': 40, u'deeplink': u'zomato://restaurant/16852773', u'id': u'16852773', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16852773_RESTAURANT_727ca2cc350b07299d7b086932c9d97b_c.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/yank-sing-soma/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/yank-sing-soma/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'303', u'aggregate_rating': u'4.1', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'SOMA', u'city_id': 306, u'country_id': 216, u'zipcode': u'94105', u'longitude': u'-122.3997194444', u'address': u'49 Stevenson Street, San Francisco 94105', u'latitude': u'37.7902222222', u'locality_verbose': u'SOMA, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/yank-sing-soma/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16852773}, u'price_range': 2, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Yank Sing', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/yank-sing-soma?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Burger, Pizza, American', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16858360_RESTAURANT_cfef899d894d38732f294c292b598ccf.jpg', u'average_cost_for_two': 20, u'deeplink': u'zomato://restaurant/16858360', u'id': u'16858360', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16858360_RESTAURANT_cfef899d894d38732f294c292b598ccf.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/wipeout-bar-grill-fishermans-wharf/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/wipeout-bar-grill-fishermans-wharf/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'114', u'aggregate_rating': u'3.7', u'rating_text': u'Good', u'rating_color': u'9ACD32'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u"Fisherman's Wharf", u'city_id': 306, u'country_id': 216, u'zipcode': u'94133', u'longitude': u'-122.4101194444', u'address': u'Pier 39, San Francisco 94133', u'latitude': u'37.8089250000', u'locality_verbose': u"Fisherman's Wharf, San Francisco"}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/wipeout-bar-grill-fishermans-wharf/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16858360}, u'price_range': 1, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Wipeout Bar &amp; Grill', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/wipeout-bar-grill-fishermans-wharf?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Mexican', u'establishment_types': [], u'currency': u'$', u'featured_image': u'', u'average_cost_for_two': 70, u'deeplink': u'zomato://restaurant/16842422', u'id': u'16842422', u'switch_to_order_menu': 0, u'thumb': u'', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/colibri-mexican-bistro-union-square/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/colibri-mexican-bistro-union-square/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'340', u'aggregate_rating': u'4.1', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Union Square', u'city_id': 306, u'country_id': 216, u'zipcode': u'94102', u'longitude': u'-122.4105444444', u'address': u'438 Geary Street, San Francisco 94102', u'latitude': u'37.7871027778', u'locality_verbose': u'Union Square, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/colibri-mexican-bistro-union-square/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16842422}, u'price_range': 3, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Colibri Mexican Bistro', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/colibri-mexican-bistro-union-square?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Seafood, Peruvian', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16853317_RESTAURANT_cd8bb8b4bdd0555ca74090358ea5c9aa_c.jpg', u'average_cost_for_two': 120, u'deeplink': u'zomato://restaurant/16853317', u'id': u'16853317', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16853317_RESTAURANT_cd8bb8b4bdd0555ca74090358ea5c9aa_c.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/la-mar-embarcadero/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/la-mar-embarcadero/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'376', u'aggregate_rating': u'4.2', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Embarcadero', u'city_id': 306, u'country_id': 216, u'zipcode': u'94111', u'longitude': u'-122.3955222222', u'address': u'Pier 1 1/2, Suite 100, San Francisco 94111', u'latitude': u'37.7971638889', u'locality_verbose': u'Embarcadero, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/la-mar-embarcadero/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16853317}, u'price_range': 4, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'La Mar', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/la-mar-embarcadero?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Seafood', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16853232_RESTAURANT_6da8a125221090cd3b6323f3455dbbd7.jpg', u'average_cost_for_two': 80, u'deeplink': u'zomato://restaurant/16853232', u'id': u'16853232', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16853232_RESTAURANT_6da8a125221090cd3b6323f3455dbbd7.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/anchor-hope-soma/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/anchor-hope-soma/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'174', u'aggregate_rating': u'3.8', u'rating_text': u'Good', u'rating_color': u'9ACD32'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'SOMA', u'city_id': 306, u'country_id': 216, u'zipcode': u'94105', u'longitude': u'-122.3990027778', u'address': u'83 Minna Street, San Francisco 94105', u'latitude': u'37.7879055556', u'locality_verbose': u'SOMA, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/anchor-hope-soma/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16853232}, u'price_range': 3, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Anchor &amp; Hope', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/anchor-hope-soma?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Italian', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16849955_RESTAURANT_f50f7046fee7aeeb7a7e1ce3252816b5.jpg', u'average_cost_for_two': 110, u'deeplink': u'zomato://restaurant/16849955', u'id': u'16849955', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16849955_RESTAURANT_f50f7046fee7aeeb7a7e1ce3252816b5.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/scalas-bistro-union-square/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/scalas-bistro-union-square/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'365', u'aggregate_rating': u'4.1', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Sir Francis Drake Hotel', u'city_id': 306, u'country_id': 216, u'zipcode': u'94102', u'longitude': u'-122.4085472222', u'address': u'Sir Francis Drake Hotel, 432 Powell Street, San Francisco 94102', u'latitude': u'37.7887500000', u'locality_verbose': u'Sir Francis Drake Hotel, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/scalas-bistro-union-square/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16849955}, u'price_range': 4, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u"Scala's Bistro", u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/scalas-bistro-union-square?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Ice Cream', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16847339_RESTAURANT_93dcb03dc77bcc34efe10c1443c51af9.png', u'average_cost_for_two': 10, u'deeplink': u'zomato://restaurant/16847339', u'id': u'16847339', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16847339_RESTAURANT_93dcb03dc77bcc34efe10c1443c51af9.png?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/mitchells-ice-cream-bernal-heights/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/mitchells-ice-cream-bernal-heights/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'580', u'aggregate_rating': u'4.7', u'rating_text': u'Excellent', u'rating_color': u'3F7E00'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Bernal Heights', u'city_id': 306, u'country_id': 216, u'zipcode': u'94110', u'longitude': u'-122.4227800000', u'address': u'688 San Jose Avenue, San Francisco 94110', u'latitude': u'37.7441970000', u'locality_verbose': u'Bernal Heights, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/mitchells-ice-cream-bernal-heights/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16847339}, u'price_range': 1, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u"Mitchell's Ice Cream", u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/mitchells-ice-cream-bernal-heights?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Burger, American', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16859437_RESTAURANT_4342f9910f781291b38322a4e49601a8_c.jpg', u'average_cost_for_two': 25, u'deeplink': u'zomato://restaurant/16859437', u'id': u'16859437', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16859437_RESTAURANT_4342f9910f781291b38322a4e49601a8_c.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/roam-artisan-burgers-cow-hollow/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/roam-artisan-burgers-cow-hollow/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'124', u'aggregate_rating': u'4.0', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Cow Hollow', u'city_id': 306, u'country_id': 216, u'zipcode': u'94123', u'longitude': u'-122.4285110000', u'address': u'1785 Union Street, San Francisco 94123', u'latitude': u'37.7978430000', u'locality_verbose': u'Cow Hollow, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/roam-artisan-burgers-cow-hollow/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16859437}, u'price_range': 1, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Roam Artisan Burgers', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/roam-artisan-burgers-cow-hollow?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Pizza, Italian', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16859729_RESTAURANT_9d83907e0a4965d22865505d8b06b8cd.jpg', u'average_cost_for_two': 65, u'deeplink': u'zomato://restaurant/16859729', u'id': u'16859729', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16859729_RESTAURANT_9d83907e0a4965d22865505d8b06b8cd.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/tonys-pizza-napoletana-north-beach/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/tonys-pizza-napoletana-north-beach/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'264', u'aggregate_rating': u'4.3', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'North Beach', u'city_id': 306, u'country_id': 216, u'zipcode': u'94133', u'longitude': u'-122.4091500000', u'address': u'1570 Stockton Street, San Francisco 94133', u'latitude': u'37.8003583333', u'locality_verbose': u'North Beach, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/tonys-pizza-napoletana-north-beach/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16859729}, u'price_range': 3, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u"Tony's Pizza Napoletana", u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/tonys-pizza-napoletana-north-beach?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Pizza', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16846393_CHAIN_c43778c2bc16df2e3e452fd524cefd69.jpg', u'average_cost_for_two': 55, u'deeplink': u'zomato://restaurant/16846394', u'id': u'16846394', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16846393_CHAIN_c43778c2bc16df2e3e452fd524cefd69.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/little-star-pizza-western-addition/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/little-star-pizza-western-addition/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'458', u'aggregate_rating': u'4.3', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Western Addition', u'city_id': 306, u'country_id': 216, u'zipcode': u'94117', u'longitude': u'-122.4384777778', u'address': u'846 Divisadero Street, San Francisco 94117', u'latitude': u'37.7775722222', u'locality_verbose': u'Western Addition, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/little-star-pizza-western-addition/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16846394}, u'price_range': 2, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Little Star Pizza', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/little-star-pizza-western-addition?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Bar Food', u'establishment_types': [], u'currency': u'$', u'featured_image': u'', u'average_cost_for_two': 45, u'deeplink': u'zomato://restaurant/16846668', u'id': u'16846668', u'switch_to_order_menu': 0, u'thumb': u'', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/magnolia-gastropub-and-brewery-haight/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/magnolia-gastropub-and-brewery-haight/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'221', u'aggregate_rating': u'4.1', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Haight', u'city_id': 306, u'country_id': 216, u'zipcode': u'94117', u'longitude': u'-122.4453277778', u'address': u'1398 Haight Street, San Francisco 94117', u'latitude': u'37.7702166667', u'locality_verbose': u'Haight, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/magnolia-gastropub-and-brewery-haight/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16846668}, u'price_range': 2, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Magnolia Gastropub And Brewery', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/magnolia-gastropub-and-brewery-haight?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Bar Food, Irish', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16857628_RESTAURANT_93c4d3ee980164b0e4cd08589e3918ff.jpg', u'average_cost_for_two': 60, u'deeplink': u'zomato://restaurant/16857628', u'id': u'16857628', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16857628_RESTAURANT_93c4d3ee980164b0e4cd08589e3918ff.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/johnny-foleys-union-square/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/johnny-foleys-union-square/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'269', u'aggregate_rating': u'4.3', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Union Square', u'city_id': 306, u'country_id': 216, u'zipcode': u'94102', u'longitude': u'-122.4088833333', u'address': u"243 O'Farrell Street, San Francisco 94102", u'latitude': u'37.7864611111', u'locality_verbose': u'Union Square, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/johnny-foleys-union-square/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16857628}, u'price_range': 3, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u"Johnny Foley's", u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/johnny-foleys-union-square?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Indian', u'establishment_types': [], u'currency': u'$', u'featured_image': u'', u'average_cost_for_two': 85, u'deeplink': u'zomato://restaurant/16857642', u'id': u'16857642', u'switch_to_order_menu': 0, u'thumb': u'', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/dosa-lower-pacific-heights/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/dosa-lower-pacific-heights/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'250', u'aggregate_rating': u'3.9', u'rating_text': u'Good', u'rating_color': u'9ACD32'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Lower Pacific Heights', u'city_id': 306, u'country_id': 216, u'zipcode': u'94115', u'longitude': u'-122.4328166667', u'address': u'1700 Fillmore Street, San Francisco 94115', u'latitude': u'37.7853388889', u'locality_verbose': u'Lower Pacific Heights, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/dosa-lower-pacific-heights/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16857642}, u'price_range': 3, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Dosa', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/dosa-lower-pacific-heights?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Thai', u'establishment_types': [], u'currency': u'$', u'featured_image': u'', u'average_cost_for_two': 40, u'deeplink': u'zomato://restaurant/16845698', u'id': u'16845698', u'switch_to_order_menu': 0, u'thumb': u'', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/king-of-thai-noodle-union-square/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/king-of-thai-noodle-union-square/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'131', u'aggregate_rating': u'3.6', u'rating_text': u'Good', u'rating_color': u'9ACD32'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Union Square', u'city_id': 306, u'country_id': 216, u'zipcode': u'94102', u'longitude': u'-122.4077833333', u'address': u"184 O'Farrell Street, San Francisco 94102", u'latitude': u'37.7864333333', u'locality_verbose': u'Union Square, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/king-of-thai-noodle-union-square/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16845698}, u'price_range': 2, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'King Of Thai Noodle', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/king-of-thai-noodle-union-square?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Mexican', u'establishment_types': [], u'currency': u'$', u'featured_image': u'', u'average_cost_for_two': 40, u'deeplink': u'zomato://restaurant/16857548', u'id': u'16857548', u'switch_to_order_menu': 0, u'thumb': u'', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/tropisue\xf1o-soma/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/tropisue\xf1o-soma/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'317', u'aggregate_rating': u'4.3', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'SOMA', u'city_id': 306, u'country_id': 216, u'zipcode': u'94103', u'longitude': u'-122.4039527778', u'address': u'75 Yerba Buena Lane, San Francisco 94103', u'latitude': u'37.7855916667', u'locality_verbose': u'SOMA, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/tropisue\xf1o-soma/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16857548}, u'price_range': 2, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Tropisue\xf1o', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/tropisue\xf1o-soma?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Seafood', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16843472_RESTAURANT_4b7580ab7c00b81bb63d33661c043ac7_c.jpg', u'average_cost_for_two': 120, u'deeplink': u'zomato://restaurant/16843472', u'id': u'16843472', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16843472_RESTAURANT_4b7580ab7c00b81bb63d33661c043ac7_c.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/farallon-nob-hill/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/farallon-nob-hill/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'286', u'aggregate_rating': u'3.9', u'rating_text': u'Good', u'rating_color': u'9ACD32'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Nob Hill', u'city_id': 306, u'country_id': 216, u'zipcode': u'94102', u'longitude': u'-122.4092320000', u'address': u'Kensington Park Hotel, First Floor, 450 Post Street, San Francisco 94102', u'latitude': u'37.7883350000', u'locality_verbose': u'Nob Hill, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/farallon-nob-hill/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16843472}, u'price_range': 4, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Farallon', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/farallon-nob-hill?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'American', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16851219_RESTAURANT_a7061f88f6daa27b2d73ea4cbf6f190c_c.jpg?output-format=webp', u'average_cost_for_two': 70, u'deeplink': u'zomato://restaurant/16851219', u'id': u'16851219', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16851219_RESTAURANT_a7061f88f6daa27b2d73ea4cbf6f190c_c.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/cliff-house-outer-richmond/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/cliff-house-outer-richmond/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'202', u'aggregate_rating': u'3.9', u'rating_text': u'Good', u'rating_color': u'9ACD32'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Outer Richmond', u'city_id': 306, u'country_id': 216, u'zipcode': u'94121', u'longitude': u'-122.5125720000', u'address': u'1090 Point Lobos Avenue, San Francisco 94121', u'latitude': u'37.7770720000', u'locality_verbose': u'Outer Richmond, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/cliff-house-outer-richmond/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16851219}, u'price_range': 3, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Cliff House', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/cliff-house-outer-richmond?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Italian, Seafood', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16842258_RESTAURANT_f16d30348353e80abced71d05d98463f.jpg', u'average_cost_for_two': 75, u'deeplink': u'zomato://restaurant/16842258', u'id': u'16842258', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16842258_RESTAURANT_f16d30348353e80abced71d05d98463f.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/cioppinos-fishermans-wharf/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/cioppinos-fishermans-wharf/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'256', u'aggregate_rating': u'3.8', u'rating_text': u'Good', u'rating_color': u'9ACD32'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u"Fisherman's Wharf", u'city_id': 306, u'country_id': 216, u'zipcode': u'94109', u'longitude': u'-122.4192972222', u'address': u'400 Jefferson Street, San Francisco 94109', u'latitude': u'37.8078472222', u'locality_verbose': u"Fisherman's Wharf, San Francisco"}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/cioppinos-fishermans-wharf/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16842258}, u'price_range': 3, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u"Cioppino's", u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/cioppinos-fishermans-wharf?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Burger, American', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16839786_CHAIN_b3f8571289cdc4ea097604ae94b43135.jpg', u'average_cost_for_two': 60, u'deeplink': u'zomato://restaurant/16839786', u'id': u'16839786', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16839786_CHAIN_b3f8571289cdc4ea097604ae94b43135.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/21st-amendment-brewery-soma/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/21st-amendment-brewery-soma/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'310', u'aggregate_rating': u'4.0', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'SOMA', u'city_id': 306, u'country_id': 216, u'zipcode': u'94107', u'longitude': u'-122.3926110000', u'address': u'563 2nd Street, San Francisco 94107', u'latitude': u'37.7824270000', u'locality_verbose': u'SOMA, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/21st-amendment-brewery-soma/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16839786}, u'price_range': 3, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'21st Amendment Brewery', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/21st-amendment-brewery-soma?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'German, American', u'establishment_types': [], u'currency': u'$', u'featured_image': u'', u'average_cost_for_two': 30, u'deeplink': u'zomato://restaurant/16852061', u'id': u'16852061', u'switch_to_order_menu': 0, u'thumb': u'', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/tommys-joynt-civic-center/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/tommys-joynt-civic-center/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'263', u'aggregate_rating': u'4.1', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Civic Center', u'city_id': 306, u'country_id': 216, u'zipcode': u'94109', u'longitude': u'-122.4218110000', u'address': u'1101 Geary Boulevard, San Francisco 94109', u'latitude': u'37.7855190000', u'locality_verbose': u'Civic Center, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/tommys-joynt-civic-center/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16852061}, u'price_range': 2, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u"Tommy's Joynt", u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/tommys-joynt-civic-center?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'American, Breakfast', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16840504_RESTAURANT_1cf63df1ee02ecc8e321ffccc2642506_c.jpg', u'average_cost_for_two': 65, u'deeplink': u'zomato://restaurant/16840504', u'id': u'16840504', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16840504_RESTAURANT_1cf63df1ee02ecc8e321ffccc2642506_c.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/bar-tartine-mission-district/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/bar-tartine-mission-district/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'240', u'aggregate_rating': u'4.0', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Mission District', u'city_id': 306, u'country_id': 216, u'zipcode': u'94110', u'longitude': u'-122.4218444444', u'address': u'561 Valencia Street, San Francisco 94110', u'latitude': u'37.7639666667', u'locality_verbose': u'Mission District, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/bar-tartine-mission-district/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16840504}, u'price_range': 3, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Bar Tartine', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/bar-tartine-mission-district?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'American, Seafood', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16843637_RESTAURANT_a1a559ead6f689981097d03b7e0d75de_c.jpg', u'average_cost_for_two': 60, u'deeplink': u'zomato://restaurant/16843637', u'id': u'16843637', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16843637_RESTAURANT_a1a559ead6f689981097d03b7e0d75de_c.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/fog-city-north-beach/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/fog-city-north-beach/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'228', u'aggregate_rating': u'4.0', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'North Beach', u'city_id': 306, u'country_id': 216, u'zipcode': u'94111', u'longitude': u'-122.4019083333', u'address': u'1300 Battery Street, San Francisco 94111', u'latitude': u'37.8036277778', u'locality_verbose': u'North Beach, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/fog-city-north-beach/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16843637}, u'price_range': 3, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Fog City', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/fog-city-north-beach?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Chinese', u'establishment_types': [], u'currency': u'$', u'featured_image': u'', u'average_cost_for_two': 45, u'deeplink': u'zomato://restaurant/16859704', u'id': u'16859704', u'switch_to_order_menu': 0, u'thumb': u'', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/mission-chinese-food-mission-district/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/mission-chinese-food-mission-district/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'200', u'aggregate_rating': u'3.9', u'rating_text': u'Good', u'rating_color': u'9ACD32'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Mission District', u'city_id': 306, u'country_id': 216, u'zipcode': u'94110', u'longitude': u'-122.4194690000', u'address': u'2234 Mission District Street, San Francisco 94110', u'latitude': u'37.7612200000', u'locality_verbose': u'Mission District, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/mission-chinese-food-mission-district/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16859704}, u'price_range': 2, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Mission Chinese Food', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/mission-chinese-food-mission-district?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Coffee and Tea', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16859109_CHAIN_e771756ca9607a718a6d5d6e081aa40e_c.png', u'average_cost_for_two': 13, u'deeplink': u'zomato://restaurant/16853142', u'id': u'16853142', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16859109_CHAIN_e771756ca9607a718a6d5d6e081aa40e_c.png?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/blue-bottle-coffee-1-soma/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/blue-bottle-coffee-1-soma/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'183', u'aggregate_rating': u'4.0', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'SOMA', u'city_id': 306, u'country_id': 216, u'zipcode': u'94103', u'longitude': u'-122.4076430000', u'address': u'66 Mint Street, San Francisco 94103', u'latitude': u'37.7823920000', u'locality_verbose': u'SOMA, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/blue-bottle-coffee-1-soma/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16853142}, u'price_range': 1, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Blue Bottle', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/blue-bottle-coffee-1-soma?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Spanish, American, Tapas', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16851889_RESTAURANT_96e0e4013b511791dd9df3f7a6766a68.jpg', u'average_cost_for_two': 50, u'deeplink': u'zomato://restaurant/16851889', u'id': u'16851889', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16851889_RESTAURANT_96e0e4013b511791dd9df3f7a6766a68.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/thirsty-bear-soma/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/thirsty-bear-soma/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'233', u'aggregate_rating': u'4.0', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'SOMA', u'city_id': 306, u'country_id': 216, u'zipcode': u'94105', u'longitude': u'-122.3999333333', u'address': u'661 Howard Street, San Francisco 94105', u'latitude': u'37.7857777778', u'locality_verbose': u'SOMA, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/thirsty-bear-soma/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16851889}, u'price_range': 2, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Thirsty Bear', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/thirsty-bear-soma?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Italian', u'establishment_types': [], u'currency': u'$', u'featured_image': u'', u'average_cost_for_two': 70, u'deeplink': u'zomato://restaurant/16848555', u'id': u'16848555', u'switch_to_order_menu': 0, u'thumb': u'', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/perbacco-financial-district/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/perbacco-financial-district/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'284', u'aggregate_rating': u'4.0', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Financial District', u'city_id': 306, u'country_id': 216, u'zipcode': u'94111', u'longitude': u'-122.3990027778', u'address': u'230 California Street, San Francisco 94111', u'latitude': u'37.7930333333', u'locality_verbose': u'Financial District, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/perbacco-financial-district/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16848555}, u'price_range': 3, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Perbacco', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/perbacco-financial-district?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Asian, Fusion', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16843051_RESTAURANT_6bfff765a701df5a9d53ef39cdb4b3f6_c.jpg', u'average_cost_for_two': 75, u'deeplink': u'zomato://restaurant/16843051', u'id': u'16843051', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16843051_RESTAURANT_6bfff765a701df5a9d53ef39cdb4b3f6_c.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/e-o-kitchen-and-bar-union-square/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/e-o-kitchen-and-bar-union-square/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'158', u'aggregate_rating': u'3.7', u'rating_text': u'Good', u'rating_color': u'9ACD32'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Union Square', u'city_id': 306, u'country_id': 216, u'zipcode': u'94108', u'longitude': u'-122.4059750000', u'address': u'314 Sutter Street, San Francisco 94108', u'latitude': u'37.7894833333', u'locality_verbose': u'Union Square, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/e-o-kitchen-and-bar-union-square/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16843051}, u'price_range': 3, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'E&amp;O Kitchen And Bar', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/e-o-kitchen-and-bar-union-square?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'American', u'establishment_types': [], u'currency': u'$', u'featured_image': u'', u'average_cost_for_two': 45, u'deeplink': u'zomato://restaurant/16846453', u'id': u'16846453', u'switch_to_order_menu': 0, u'thumb': u'', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/loris-diner-union-square/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/loris-diner-union-square/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'149', u'aggregate_rating': u'3.6', u'rating_text': u'Good', u'rating_color': u'9ACD32'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Union Square', u'city_id': 306, u'country_id': 216, u'zipcode': u'94102', u'longitude': u'-122.4088500000', u'address': u'500 Sutter St,Suite 708, San Francisco 94102', u'latitude': u'37.7893780000', u'locality_verbose': u'Union Square, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/loris-diner-union-square/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16846453}, u'price_range': 2, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u"Lori's Diner", u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/loris-diner-union-square?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'California, French', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16852939_RESTAURANT_2a66fda8616f5beb0e66a1b2ae53d418.png', u'average_cost_for_two': 80, u'deeplink': u'zomato://restaurant/16852939', u'id': u'16852939', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16852939_RESTAURANT_2a66fda8616f5beb0e66a1b2ae53d418.png?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/zazie-cole-valley/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/zazie-cole-valley/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'355', u'aggregate_rating': u'4.2', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Cole Valley', u'city_id': 306, u'country_id': 216, u'zipcode': u'94117', u'longitude': u'-122.4500277778', u'address': u'941 Cole Street, San Francisco 94117', u'latitude': u'37.7653083333', u'locality_verbose': u'Cole Valley, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/zazie-cole-valley/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16852939}, u'price_range': 3, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Zazie', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/zazie-cole-valley?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Indian', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16853336_RESTAURANT_9ed39529bf42cd768a34328de864fa21_c.jpg', u'average_cost_for_two': 80, u'deeplink': u'zomato://restaurant/16853336', u'id': u'16853336', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16853336_RESTAURANT_9ed39529bf42cd768a34328de864fa21_c.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/amber-soma/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/amber-soma/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'279', u'aggregate_rating': u'4.1', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'SOMA', u'city_id': 306, u'country_id': 216, u'zipcode': u'94103', u'longitude': u'-122.4045598000', u'address': u'25 Yerba Buena Lane, San Francisco 94103', u'latitude': u'37.7858492000', u'locality_verbose': u'SOMA, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/amber-soma/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16853336}, u'price_range': 3, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Amber', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/amber-soma?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'American, California', u'establishment_types': [], u'currency': u'$', u'featured_image': u'', u'average_cost_for_two': 80, u'deeplink': u'zomato://restaurant/16849242', u'id': u'16849242', u'switch_to_order_menu': 0, u'thumb': u'', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/range-mission-district/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/range-mission-district/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'447', u'aggregate_rating': u'4.1', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Mission District', u'city_id': 306, u'country_id': 216, u'zipcode': u'94110', u'longitude': u'-122.4214555556', u'address': u'842 Valencia Street, San Francisco 94110', u'latitude': u'37.7594305556', u'locality_verbose': u'Mission District, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/range-mission-district/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16849242}, u'price_range': 3, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Range', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/range-mission-district?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Italian', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16853088_RESTAURANT_03097a5fa95650c739de0e8f4366cc07_c.jpg', u'average_cost_for_two': 115, u'deeplink': u'zomato://restaurant/16853088', u'id': u'16853088', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16853088_RESTAURANT_03097a5fa95650c739de0e8f4366cc07_c.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/spqr-lower-pacific-heights/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/spqr-lower-pacific-heights/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'345', u'aggregate_rating': u'4.1', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Lower Pacific Heights', u'city_id': 306, u'country_id': 216, u'zipcode': u'94115', u'longitude': u'-122.4335722222', u'address': u'1911 Fillmore Street,  San Francisco 94115', u'latitude': u'37.7873527778', u'locality_verbose': u'Lower Pacific Heights, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/spqr-lower-pacific-heights/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16853088}, u'price_range': 4, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'SPQR', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/spqr-lower-pacific-heights?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Mexican', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16844174_RESTAURANT_c655b037649ab19d5c1d3e689cac63e7_c.jpg', u'average_cost_for_two': 65, u'deeplink': u'zomato://restaurant/16844174', u'id': u'16844174', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16844174_RESTAURANT_c655b037649ab19d5c1d3e689cac63e7_c.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/green-chile-kitchen-western-addition/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/green-chile-kitchen-western-addition/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'189', u'aggregate_rating': u'4.3', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Western Addition', u'city_id': 306, u'country_id': 216, u'zipcode': u'94115', u'longitude': u'-122.4419861111', u'address': u'1801 McAllister Street, San Francisco 94115', u'latitude': u'37.7773694444', u'locality_verbose': u'Western Addition, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/green-chile-kitchen-western-addition/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16844174}, u'price_range': 3, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Green Chile Kitchen', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/green-chile-kitchen-western-addition?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'American', u'establishment_types': [], u'currency': u'$', u'featured_image': u'', u'average_cost_for_two': 110, u'deeplink': u'zomato://restaurant/16852137', u'id': u'16852137', u'switch_to_order_menu': 0, u'thumb': u'', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/town-hall-financial-district/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/town-hall-financial-district/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'293', u'aggregate_rating': u'4.0', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Financial District', u'city_id': 306, u'country_id': 216, u'zipcode': u'94105', u'longitude': u'-122.3947860000', u'address': u'342 Howard Street, San Francisco 94105', u'latitude': u'37.7896790000', u'locality_verbose': u'Financial District, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/town-hall-financial-district/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16852137}, u'price_range': 4, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Town Hall', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/town-hall-financial-district?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Japanese, Sushi', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16848139_RESTAURANT_88a81a2ae3bd6c1de037e47f5524f1bf_c.jpg', u'average_cost_for_two': 50, u'deeplink': u'zomato://restaurant/16848139', u'id': u'16848139', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16848139_RESTAURANT_88a81a2ae3bd6c1de037e47f5524f1bf_c.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/ozumo-financial-district/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/ozumo-financial-district/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'298', u'aggregate_rating': u'3.9', u'rating_text': u'Good', u'rating_color': u'9ACD32'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Financial District', u'city_id': 306, u'country_id': 216, u'zipcode': u'94105', u'longitude': u'-122.3922811000', u'address': u'161 Steuart Street, San Francisco 94105', u'latitude': u'37.7926743000', u'locality_verbose': u'Financial District, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/ozumo-financial-district/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16848139}, u'price_range': 2, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Ozumo', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/ozumo-financial-district?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Seafood, American', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16846955_RESTAURANT_b0ae7754ab157e5620bf944e7007032d_c.jpg', u'average_cost_for_two': 65, u'deeplink': u'zomato://restaurant/16846955', u'id': u'16846955', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16846955_RESTAURANT_b0ae7754ab157e5620bf944e7007032d_c.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/mccormick-kuletos-fishermans-wharf/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/mccormick-kuletos-fishermans-wharf/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'246', u'aggregate_rating': u'3.8', u'rating_text': u'Good', u'rating_color': u'9ACD32'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Ghiradelli Square', u'city_id': 306, u'country_id': 216, u'zipcode': u'94109', u'longitude': u'-122.4223027778', u'address': u'Ghirardelli Square, 900 North Point Street, San Francisco 94109', u'latitude': u'37.8061972222', u'locality_verbose': u'Ghiradelli Square, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/mccormick-kuletos-fishermans-wharf/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16846955}, u'price_range': 3, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u"McCormick &amp; Kuleto's", u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/mccormick-kuletos-fishermans-wharf?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'Tapas, Spanish', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16862108_RESTAURANT_917a76df4b946e9a3291f3a5dea6ea44.jpg', u'average_cost_for_two': 70, u'deeplink': u'zomato://restaurant/16862108', u'id': u'16862108', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16862108_RESTAURANT_917a76df4b946e9a3291f3a5dea6ea44.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/coqueta-embarcadero/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/coqueta-embarcadero/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'94', u'aggregate_rating': u'3.6', u'rating_text': u'Good', u'rating_color': u'9ACD32'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Embarcadero', u'city_id': 306, u'country_id': 216, u'zipcode': u'94105', u'longitude': u'-122.3966611111', u'address': u'Pier 5, San Francisco 94105', u'latitude': u'37.7985222222', u'locality_verbose': u'Embarcadero, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/coqueta-embarcadero/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16862108}, u'price_range': 3, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Coqueta', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/coqueta-embarcadero?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'American', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16840830_RESTAURANT_797ad6d251817aad8b4b364bd0b8f357.jpg', u'average_cost_for_two': 0, u'deeplink': u'zomato://restaurant/16840830', u'id': u'16840830', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16840830_RESTAURANT_797ad6d251817aad8b4b364bd0b8f357.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/bix-financial-district/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/bix-financial-district/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'232', u'aggregate_rating': u'4.2', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Financial District', u'city_id': 306, u'country_id': 216, u'zipcode': u'94133', u'longitude': u'-122.4028388889', u'address': u'56 Gold Street, San Francisco 94133', u'latitude': u'37.7967916667', u'locality_verbose': u'Financial District, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/bix-financial-district/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16840830}, u'price_range': 1, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Bix', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/bix-financial-district?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
+  <si>
+    <t>{u'restaurant': {u'cuisines': u'French', u'establishment_types': [], u'currency': u'$', u'featured_image': u'https://b.zmtcdn.com/data/res_imagery/16841329_RESTAURANT_d81e1981a3d5058557ccd45c8be04964_c.jpg', u'average_cost_for_two': 75, u'deeplink': u'zomato://restaurant/16841329', u'id': u'16841329', u'switch_to_order_menu': 0, u'thumb': u'https://b.zmtcdn.com/data/res_imagery/16841329_RESTAURANT_d81e1981a3d5058557ccd45c8be04964_c.jpg?fit=around%7C200%3A200&amp;crop=200%3A200%3B%2A%2C%2A', u'is_delivering_now': 0, u'menu_url': u'https://www.zomato.com/san-francisco/cafe-claude-union-square/menu?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1&amp;openSwipeBox=menu&amp;showMinimal=1#tabtop', u'photos_url': u'https://www.zomato.com/san-francisco/cafe-claude-union-square/photos?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1#tabtop', u'user_rating': {u'votes': u'222', u'aggregate_rating': u'4.2', u'rating_text': u'Very Good', u'rating_color': u'5BA829'}, u'offers': [], u'location': {u'city': u'San Francisco', u'locality': u'Union Square', u'city_id': 306, u'country_id': 216, u'zipcode': u'94108', u'longitude': u'-122.4041750000', u'address': u'7 Claude Lane, San Francisco 94108', u'latitude': u'37.7901916667', u'locality_verbose': u'Union Square, San Francisco'}, u'has_table_booking': 0, u'events_url': u'https://www.zomato.com/san-francisco/cafe-claude-union-square/events#tabtop?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1', u'R': {u'res_id': 16841329}, u'price_range': 3, u'apikey': u'592789033e4cf0e384b54c1ec424c706', u'name': u'Cafe Claude', u'has_online_delivery': 0, u'url': u'https://www.zomato.com/san-francisco/cafe-claude-union-square?utm_source=api_basic_user&amp;utm_medium=api&amp;utm_campaign=v2.1'}}</t>
+  </si>
   <si>
     <t>Rating</t>
   </si>
@@ -1016,1424 +1320,1942 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D101"/>
+  <dimension ref="A1:A101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1">
+      <c r="A95" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101" t="s">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D101"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>101</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>103</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>120</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>123</v>
       </c>
       <c r="D2" t="s">
-        <v>120</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>106</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>120</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>124</v>
       </c>
       <c r="D3" t="s">
-        <v>121</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>107</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>125</v>
       </c>
       <c r="D4" t="s">
-        <v>122</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>106</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>120</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>126</v>
       </c>
       <c r="D5" t="s">
-        <v>123</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>108</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>120</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>127</v>
       </c>
       <c r="D6" t="s">
-        <v>124</v>
+        <v>225</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>109</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>128</v>
       </c>
       <c r="D7" t="s">
-        <v>125</v>
+        <v>226</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>110</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>129</v>
       </c>
       <c r="D8" t="s">
-        <v>126</v>
+        <v>227</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>111</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>130</v>
       </c>
       <c r="D9" t="s">
-        <v>127</v>
+        <v>228</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>109</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>131</v>
       </c>
       <c r="D10" t="s">
-        <v>128</v>
+        <v>229</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>109</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>132</v>
       </c>
       <c r="D11" t="s">
-        <v>129</v>
+        <v>230</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>112</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>122</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>133</v>
       </c>
       <c r="D12" t="s">
-        <v>130</v>
+        <v>231</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>105</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>120</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>134</v>
       </c>
       <c r="D13" t="s">
-        <v>131</v>
+        <v>232</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>110</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>135</v>
       </c>
       <c r="D14" t="s">
-        <v>132</v>
+        <v>233</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>107</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C15" t="s">
-        <v>35</v>
+        <v>136</v>
       </c>
       <c r="D15" t="s">
-        <v>133</v>
+        <v>234</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>108</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>120</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
+        <v>137</v>
       </c>
       <c r="D16" t="s">
-        <v>134</v>
+        <v>235</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>106</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>120</v>
       </c>
       <c r="C17" t="s">
-        <v>37</v>
+        <v>138</v>
       </c>
       <c r="D17" t="s">
-        <v>135</v>
+        <v>236</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>113</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>120</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
+        <v>139</v>
       </c>
       <c r="D18" t="s">
-        <v>136</v>
+        <v>237</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>110</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
+        <v>140</v>
       </c>
       <c r="D19" t="s">
-        <v>137</v>
+        <v>238</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>6</v>
+        <v>107</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>141</v>
       </c>
       <c r="D20" t="s">
-        <v>138</v>
+        <v>239</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>114</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>142</v>
       </c>
       <c r="D21" t="s">
-        <v>139</v>
+        <v>240</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>8</v>
+        <v>109</v>
       </c>
       <c r="B22" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C22" t="s">
-        <v>42</v>
+        <v>143</v>
       </c>
       <c r="D22" t="s">
-        <v>140</v>
+        <v>241</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>115</v>
       </c>
       <c r="B23" t="s">
-        <v>19</v>
+        <v>120</v>
       </c>
       <c r="C23" t="s">
-        <v>43</v>
+        <v>144</v>
       </c>
       <c r="D23" t="s">
-        <v>134</v>
+        <v>235</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>6</v>
+        <v>107</v>
       </c>
       <c r="B24" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C24" t="s">
-        <v>44</v>
+        <v>145</v>
       </c>
       <c r="D24" t="s">
-        <v>141</v>
+        <v>242</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>8</v>
+        <v>109</v>
       </c>
       <c r="B25" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C25" t="s">
-        <v>45</v>
+        <v>146</v>
       </c>
       <c r="D25" t="s">
-        <v>142</v>
+        <v>243</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>8</v>
+        <v>109</v>
       </c>
       <c r="B26" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C26" t="s">
-        <v>46</v>
+        <v>147</v>
       </c>
       <c r="D26" t="s">
-        <v>143</v>
+        <v>244</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>10</v>
+        <v>111</v>
       </c>
       <c r="B27" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C27" t="s">
-        <v>47</v>
+        <v>148</v>
       </c>
       <c r="D27" t="s">
-        <v>144</v>
+        <v>245</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>10</v>
+        <v>111</v>
       </c>
       <c r="B28" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C28" t="s">
-        <v>48</v>
+        <v>149</v>
       </c>
       <c r="D28" t="s">
-        <v>145</v>
+        <v>246</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>6</v>
+        <v>107</v>
       </c>
       <c r="B29" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C29" t="s">
-        <v>49</v>
+        <v>150</v>
       </c>
       <c r="D29" t="s">
-        <v>146</v>
+        <v>247</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>8</v>
+        <v>109</v>
       </c>
       <c r="B30" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C30" t="s">
-        <v>50</v>
+        <v>151</v>
       </c>
       <c r="D30" t="s">
-        <v>147</v>
+        <v>248</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>10</v>
+        <v>111</v>
       </c>
       <c r="B31" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C31" t="s">
-        <v>51</v>
+        <v>152</v>
       </c>
       <c r="D31" t="s">
-        <v>148</v>
+        <v>249</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>10</v>
+        <v>111</v>
       </c>
       <c r="B32" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C32" t="s">
-        <v>52</v>
+        <v>153</v>
       </c>
       <c r="D32" t="s">
-        <v>149</v>
+        <v>250</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>5</v>
+        <v>106</v>
       </c>
       <c r="B33" t="s">
-        <v>19</v>
+        <v>120</v>
       </c>
       <c r="C33" t="s">
-        <v>53</v>
+        <v>154</v>
       </c>
       <c r="D33" t="s">
-        <v>150</v>
+        <v>251</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>8</v>
+        <v>109</v>
       </c>
       <c r="B34" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C34" t="s">
-        <v>54</v>
+        <v>155</v>
       </c>
       <c r="D34" t="s">
-        <v>151</v>
+        <v>252</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>14</v>
+        <v>115</v>
       </c>
       <c r="B35" t="s">
-        <v>19</v>
+        <v>120</v>
       </c>
       <c r="C35" t="s">
-        <v>55</v>
+        <v>156</v>
       </c>
       <c r="D35" t="s">
-        <v>152</v>
+        <v>253</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>8</v>
+        <v>109</v>
       </c>
       <c r="B36" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C36" t="s">
-        <v>56</v>
+        <v>157</v>
       </c>
       <c r="D36" t="s">
-        <v>153</v>
+        <v>254</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>8</v>
+        <v>109</v>
       </c>
       <c r="B37" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C37" t="s">
-        <v>57</v>
+        <v>158</v>
       </c>
       <c r="D37" t="s">
-        <v>154</v>
+        <v>255</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>13</v>
+        <v>114</v>
       </c>
       <c r="B38" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C38" t="s">
-        <v>58</v>
+        <v>159</v>
       </c>
       <c r="D38" t="s">
-        <v>155</v>
+        <v>256</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>5</v>
+        <v>106</v>
       </c>
       <c r="B39" t="s">
-        <v>19</v>
+        <v>120</v>
       </c>
       <c r="C39" t="s">
-        <v>59</v>
+        <v>160</v>
       </c>
       <c r="D39" t="s">
-        <v>156</v>
+        <v>257</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>8</v>
+        <v>109</v>
       </c>
       <c r="B40" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C40" t="s">
-        <v>60</v>
+        <v>161</v>
       </c>
       <c r="D40" t="s">
-        <v>157</v>
+        <v>258</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>5</v>
+        <v>106</v>
       </c>
       <c r="B41" t="s">
-        <v>19</v>
+        <v>120</v>
       </c>
       <c r="C41" t="s">
-        <v>61</v>
+        <v>162</v>
       </c>
       <c r="D41" t="s">
-        <v>158</v>
+        <v>259</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>13</v>
+        <v>114</v>
       </c>
       <c r="B42" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C42" t="s">
-        <v>62</v>
+        <v>163</v>
       </c>
       <c r="D42" t="s">
-        <v>159</v>
+        <v>260</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>7</v>
+        <v>108</v>
       </c>
       <c r="B43" t="s">
-        <v>19</v>
+        <v>120</v>
       </c>
       <c r="C43" t="s">
-        <v>63</v>
+        <v>164</v>
       </c>
       <c r="D43" t="s">
-        <v>160</v>
+        <v>261</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>9</v>
+        <v>110</v>
       </c>
       <c r="B44" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C44" t="s">
-        <v>64</v>
+        <v>165</v>
       </c>
       <c r="D44" t="s">
-        <v>161</v>
+        <v>262</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>6</v>
+        <v>107</v>
       </c>
       <c r="B45" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C45" t="s">
-        <v>65</v>
+        <v>166</v>
       </c>
       <c r="D45" t="s">
-        <v>162</v>
+        <v>263</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>8</v>
+        <v>109</v>
       </c>
       <c r="B46" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C46" t="s">
-        <v>66</v>
+        <v>167</v>
       </c>
       <c r="D46" t="s">
-        <v>163</v>
+        <v>264</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>10</v>
+        <v>111</v>
       </c>
       <c r="B47" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C47" t="s">
-        <v>67</v>
+        <v>168</v>
       </c>
       <c r="D47" t="s">
-        <v>164</v>
+        <v>265</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>9</v>
+        <v>110</v>
       </c>
       <c r="B48" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C48" t="s">
-        <v>68</v>
+        <v>169</v>
       </c>
       <c r="D48" t="s">
-        <v>165</v>
+        <v>266</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>6</v>
+        <v>107</v>
       </c>
       <c r="B49" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C49" t="s">
-        <v>69</v>
+        <v>170</v>
       </c>
       <c r="D49" t="s">
-        <v>166</v>
+        <v>267</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>10</v>
+        <v>111</v>
       </c>
       <c r="B50" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C50" t="s">
-        <v>70</v>
+        <v>171</v>
       </c>
       <c r="D50" t="s">
-        <v>167</v>
+        <v>268</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>15</v>
+        <v>116</v>
       </c>
       <c r="B51" t="s">
-        <v>21</v>
+        <v>122</v>
       </c>
       <c r="C51" t="s">
-        <v>71</v>
+        <v>172</v>
       </c>
       <c r="D51" t="s">
-        <v>168</v>
+        <v>269</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>6</v>
+        <v>107</v>
       </c>
       <c r="B52" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C52" t="s">
-        <v>72</v>
+        <v>173</v>
       </c>
       <c r="D52" t="s">
-        <v>169</v>
+        <v>270</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>6</v>
+        <v>107</v>
       </c>
       <c r="B53" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C53" t="s">
-        <v>73</v>
+        <v>174</v>
       </c>
       <c r="D53" t="s">
-        <v>170</v>
+        <v>271</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>10</v>
+        <v>111</v>
       </c>
       <c r="B54" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C54" t="s">
-        <v>74</v>
+        <v>175</v>
       </c>
       <c r="D54" t="s">
-        <v>171</v>
+        <v>272</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>16</v>
+        <v>117</v>
       </c>
       <c r="B55" t="s">
-        <v>21</v>
+        <v>122</v>
       </c>
       <c r="C55" t="s">
-        <v>75</v>
+        <v>176</v>
       </c>
       <c r="D55" t="s">
-        <v>172</v>
+        <v>273</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>11</v>
+        <v>112</v>
       </c>
       <c r="B56" t="s">
-        <v>21</v>
+        <v>122</v>
       </c>
       <c r="C56" t="s">
-        <v>76</v>
+        <v>177</v>
       </c>
       <c r="D56" t="s">
-        <v>173</v>
+        <v>274</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>6</v>
+        <v>107</v>
       </c>
       <c r="B57" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C57" t="s">
-        <v>77</v>
+        <v>178</v>
       </c>
       <c r="D57" t="s">
-        <v>174</v>
+        <v>275</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>9</v>
+        <v>110</v>
       </c>
       <c r="B58" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C58" t="s">
-        <v>78</v>
+        <v>179</v>
       </c>
       <c r="D58" t="s">
-        <v>175</v>
+        <v>276</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>15</v>
+        <v>116</v>
       </c>
       <c r="B59" t="s">
-        <v>21</v>
+        <v>122</v>
       </c>
       <c r="C59" t="s">
-        <v>79</v>
+        <v>180</v>
       </c>
       <c r="D59" t="s">
-        <v>176</v>
+        <v>277</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>17</v>
+        <v>118</v>
       </c>
       <c r="B60" t="s">
-        <v>21</v>
+        <v>122</v>
       </c>
       <c r="C60" t="s">
-        <v>80</v>
+        <v>181</v>
       </c>
       <c r="D60" t="s">
-        <v>177</v>
+        <v>278</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>11</v>
+        <v>112</v>
       </c>
       <c r="B61" t="s">
-        <v>21</v>
+        <v>122</v>
       </c>
       <c r="C61" t="s">
-        <v>81</v>
+        <v>182</v>
       </c>
       <c r="D61" t="s">
-        <v>146</v>
+        <v>247</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>7</v>
+        <v>108</v>
       </c>
       <c r="B62" t="s">
-        <v>19</v>
+        <v>120</v>
       </c>
       <c r="C62" t="s">
-        <v>82</v>
+        <v>183</v>
       </c>
       <c r="D62" t="s">
-        <v>178</v>
+        <v>279</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>13</v>
+        <v>114</v>
       </c>
       <c r="B63" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C63" t="s">
-        <v>83</v>
+        <v>184</v>
       </c>
       <c r="D63" t="s">
-        <v>179</v>
+        <v>280</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>15</v>
+        <v>116</v>
       </c>
       <c r="B64" t="s">
-        <v>21</v>
+        <v>122</v>
       </c>
       <c r="C64" t="s">
-        <v>84</v>
+        <v>185</v>
       </c>
       <c r="D64" t="s">
-        <v>180</v>
+        <v>281</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>13</v>
+        <v>114</v>
       </c>
       <c r="B65" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C65" t="s">
-        <v>85</v>
+        <v>186</v>
       </c>
       <c r="D65" t="s">
-        <v>181</v>
+        <v>282</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>9</v>
+        <v>110</v>
       </c>
       <c r="B66" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C66" t="s">
-        <v>86</v>
+        <v>187</v>
       </c>
       <c r="D66" t="s">
-        <v>182</v>
+        <v>283</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>16</v>
+        <v>117</v>
       </c>
       <c r="B67" t="s">
-        <v>21</v>
+        <v>122</v>
       </c>
       <c r="C67" t="s">
-        <v>87</v>
+        <v>188</v>
       </c>
       <c r="D67" t="s">
-        <v>183</v>
+        <v>284</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>13</v>
+        <v>114</v>
       </c>
       <c r="B68" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C68" t="s">
-        <v>88</v>
+        <v>189</v>
       </c>
       <c r="D68" t="s">
-        <v>184</v>
+        <v>285</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
-        <v>14</v>
+        <v>115</v>
       </c>
       <c r="B69" t="s">
-        <v>19</v>
+        <v>120</v>
       </c>
       <c r="C69" t="s">
-        <v>89</v>
+        <v>190</v>
       </c>
       <c r="D69" t="s">
-        <v>185</v>
+        <v>286</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" t="s">
-        <v>10</v>
+        <v>111</v>
       </c>
       <c r="B70" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C70" t="s">
-        <v>90</v>
+        <v>191</v>
       </c>
       <c r="D70" t="s">
-        <v>186</v>
+        <v>287</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" t="s">
-        <v>6</v>
+        <v>107</v>
       </c>
       <c r="B71" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C71" t="s">
-        <v>91</v>
+        <v>192</v>
       </c>
       <c r="D71" t="s">
-        <v>187</v>
+        <v>288</v>
       </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" t="s">
-        <v>6</v>
+        <v>107</v>
       </c>
       <c r="B72" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C72" t="s">
-        <v>92</v>
+        <v>193</v>
       </c>
       <c r="D72" t="s">
-        <v>188</v>
+        <v>289</v>
       </c>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" t="s">
-        <v>13</v>
+        <v>114</v>
       </c>
       <c r="B73" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C73" t="s">
-        <v>93</v>
+        <v>194</v>
       </c>
       <c r="D73" t="s">
-        <v>189</v>
+        <v>290</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" t="s">
-        <v>6</v>
+        <v>107</v>
       </c>
       <c r="B74" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C74" t="s">
-        <v>94</v>
+        <v>195</v>
       </c>
       <c r="D74" t="s">
-        <v>190</v>
+        <v>291</v>
       </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" t="s">
-        <v>11</v>
+        <v>112</v>
       </c>
       <c r="B75" t="s">
-        <v>21</v>
+        <v>122</v>
       </c>
       <c r="C75" t="s">
-        <v>78</v>
+        <v>179</v>
       </c>
       <c r="D75" t="s">
-        <v>191</v>
+        <v>292</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" t="s">
-        <v>18</v>
+        <v>119</v>
       </c>
       <c r="B76" t="s">
-        <v>21</v>
+        <v>122</v>
       </c>
       <c r="C76" t="s">
-        <v>95</v>
+        <v>196</v>
       </c>
       <c r="D76" t="s">
-        <v>192</v>
+        <v>293</v>
       </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" t="s">
-        <v>6</v>
+        <v>107</v>
       </c>
       <c r="B77" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C77" t="s">
-        <v>96</v>
+        <v>197</v>
       </c>
       <c r="D77" t="s">
-        <v>193</v>
+        <v>294</v>
       </c>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" t="s">
-        <v>11</v>
+        <v>112</v>
       </c>
       <c r="B78" t="s">
-        <v>21</v>
+        <v>122</v>
       </c>
       <c r="C78" t="s">
-        <v>97</v>
+        <v>198</v>
       </c>
       <c r="D78" t="s">
-        <v>139</v>
+        <v>240</v>
       </c>
     </row>
     <row r="79" spans="1:4">
       <c r="A79" t="s">
-        <v>11</v>
+        <v>112</v>
       </c>
       <c r="B79" t="s">
-        <v>21</v>
+        <v>122</v>
       </c>
       <c r="C79" t="s">
-        <v>98</v>
+        <v>199</v>
       </c>
       <c r="D79" t="s">
-        <v>194</v>
+        <v>295</v>
       </c>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" t="s">
-        <v>16</v>
+        <v>117</v>
       </c>
       <c r="B80" t="s">
-        <v>21</v>
+        <v>122</v>
       </c>
       <c r="C80" t="s">
-        <v>99</v>
+        <v>200</v>
       </c>
       <c r="D80" t="s">
-        <v>195</v>
+        <v>296</v>
       </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" t="s">
-        <v>10</v>
+        <v>111</v>
       </c>
       <c r="B81" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C81" t="s">
-        <v>100</v>
+        <v>201</v>
       </c>
       <c r="D81" t="s">
-        <v>159</v>
+        <v>260</v>
       </c>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" t="s">
-        <v>13</v>
+        <v>114</v>
       </c>
       <c r="B82" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C82" t="s">
-        <v>101</v>
+        <v>202</v>
       </c>
       <c r="D82" t="s">
-        <v>196</v>
+        <v>297</v>
       </c>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" t="s">
-        <v>10</v>
+        <v>111</v>
       </c>
       <c r="B83" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C83" t="s">
-        <v>102</v>
+        <v>203</v>
       </c>
       <c r="D83" t="s">
-        <v>197</v>
+        <v>298</v>
       </c>
     </row>
     <row r="84" spans="1:4">
       <c r="A84" t="s">
-        <v>10</v>
+        <v>111</v>
       </c>
       <c r="B84" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C84" t="s">
-        <v>103</v>
+        <v>204</v>
       </c>
       <c r="D84" t="s">
-        <v>198</v>
+        <v>299</v>
       </c>
     </row>
     <row r="85" spans="1:4">
       <c r="A85" t="s">
-        <v>11</v>
+        <v>112</v>
       </c>
       <c r="B85" t="s">
-        <v>21</v>
+        <v>122</v>
       </c>
       <c r="C85" t="s">
-        <v>104</v>
+        <v>205</v>
       </c>
       <c r="D85" t="s">
-        <v>199</v>
+        <v>300</v>
       </c>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" t="s">
-        <v>10</v>
+        <v>111</v>
       </c>
       <c r="B86" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C86" t="s">
-        <v>76</v>
+        <v>177</v>
       </c>
       <c r="D86" t="s">
-        <v>176</v>
+        <v>277</v>
       </c>
     </row>
     <row r="87" spans="1:4">
       <c r="A87" t="s">
-        <v>10</v>
+        <v>111</v>
       </c>
       <c r="B87" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C87" t="s">
-        <v>105</v>
+        <v>206</v>
       </c>
       <c r="D87" t="s">
-        <v>200</v>
+        <v>301</v>
       </c>
     </row>
     <row r="88" spans="1:4">
       <c r="A88" t="s">
-        <v>10</v>
+        <v>111</v>
       </c>
       <c r="B88" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C88" t="s">
-        <v>106</v>
+        <v>207</v>
       </c>
       <c r="D88" t="s">
-        <v>201</v>
+        <v>302</v>
       </c>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" t="s">
-        <v>15</v>
+        <v>116</v>
       </c>
       <c r="B89" t="s">
-        <v>21</v>
+        <v>122</v>
       </c>
       <c r="C89" t="s">
-        <v>107</v>
+        <v>208</v>
       </c>
       <c r="D89" t="s">
-        <v>202</v>
+        <v>303</v>
       </c>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" t="s">
-        <v>18</v>
+        <v>119</v>
       </c>
       <c r="B90" t="s">
-        <v>21</v>
+        <v>122</v>
       </c>
       <c r="C90" t="s">
-        <v>108</v>
+        <v>209</v>
       </c>
       <c r="D90" t="s">
-        <v>203</v>
+        <v>304</v>
       </c>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" t="s">
-        <v>9</v>
+        <v>110</v>
       </c>
       <c r="B91" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C91" t="s">
-        <v>109</v>
+        <v>210</v>
       </c>
       <c r="D91" t="s">
-        <v>204</v>
+        <v>305</v>
       </c>
     </row>
     <row r="92" spans="1:4">
       <c r="A92" t="s">
-        <v>13</v>
+        <v>114</v>
       </c>
       <c r="B92" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C92" t="s">
-        <v>110</v>
+        <v>211</v>
       </c>
       <c r="D92" t="s">
-        <v>205</v>
+        <v>306</v>
       </c>
     </row>
     <row r="93" spans="1:4">
       <c r="A93" t="s">
-        <v>13</v>
+        <v>114</v>
       </c>
       <c r="B93" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C93" t="s">
-        <v>111</v>
+        <v>212</v>
       </c>
       <c r="D93" t="s">
-        <v>206</v>
+        <v>307</v>
       </c>
     </row>
     <row r="94" spans="1:4">
       <c r="A94" t="s">
-        <v>13</v>
+        <v>114</v>
       </c>
       <c r="B94" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C94" t="s">
-        <v>112</v>
+        <v>213</v>
       </c>
       <c r="D94" t="s">
-        <v>207</v>
+        <v>308</v>
       </c>
     </row>
     <row r="95" spans="1:4">
       <c r="A95" t="s">
-        <v>6</v>
+        <v>107</v>
       </c>
       <c r="B95" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C95" t="s">
-        <v>113</v>
+        <v>214</v>
       </c>
       <c r="D95" t="s">
-        <v>208</v>
+        <v>309</v>
       </c>
     </row>
     <row r="96" spans="1:4">
       <c r="A96" t="s">
-        <v>10</v>
+        <v>111</v>
       </c>
       <c r="B96" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C96" t="s">
-        <v>114</v>
+        <v>215</v>
       </c>
       <c r="D96" t="s">
-        <v>209</v>
+        <v>310</v>
       </c>
     </row>
     <row r="97" spans="1:4">
       <c r="A97" t="s">
-        <v>11</v>
+        <v>112</v>
       </c>
       <c r="B97" t="s">
-        <v>21</v>
+        <v>122</v>
       </c>
       <c r="C97" t="s">
-        <v>115</v>
+        <v>216</v>
       </c>
       <c r="D97" t="s">
-        <v>210</v>
+        <v>311</v>
       </c>
     </row>
     <row r="98" spans="1:4">
       <c r="A98" t="s">
-        <v>16</v>
+        <v>117</v>
       </c>
       <c r="B98" t="s">
-        <v>21</v>
+        <v>122</v>
       </c>
       <c r="C98" t="s">
-        <v>116</v>
+        <v>217</v>
       </c>
       <c r="D98" t="s">
-        <v>211</v>
+        <v>312</v>
       </c>
     </row>
     <row r="99" spans="1:4">
       <c r="A99" t="s">
-        <v>18</v>
+        <v>119</v>
       </c>
       <c r="B99" t="s">
-        <v>21</v>
+        <v>122</v>
       </c>
       <c r="C99" t="s">
-        <v>117</v>
+        <v>218</v>
       </c>
       <c r="D99" t="s">
-        <v>212</v>
+        <v>313</v>
       </c>
     </row>
     <row r="100" spans="1:4">
       <c r="A100" t="s">
-        <v>9</v>
+        <v>110</v>
       </c>
       <c r="B100" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C100" t="s">
-        <v>118</v>
+        <v>219</v>
       </c>
       <c r="D100" t="s">
-        <v>213</v>
+        <v>314</v>
       </c>
     </row>
     <row r="101" spans="1:4">
       <c r="A101" t="s">
-        <v>9</v>
+        <v>110</v>
       </c>
       <c r="B101" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C101" t="s">
-        <v>119</v>
+        <v>220</v>
       </c>
       <c r="D101" t="s">
-        <v>214</v>
+        <v>315</v>
       </c>
     </row>
   </sheetData>

</xml_diff>